<commit_message>
Insure Report, TempSalary & MySuccess Update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15D399-5D88-4EDA-B262-864898128B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9789CDBF-BB03-4C32-A480-4279C67D5038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,10 +250,10 @@
     <t>She Macc Lite</t>
   </si>
   <si>
-    <t>Cancer Lite</t>
-  </si>
-  <si>
-    <t>Macc Lite</t>
+    <t>Macc Fun R99</t>
+  </si>
+  <si>
+    <t>Cancer R99</t>
   </si>
 </sst>
 </file>
@@ -1075,6 +1075,39 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1091,39 +1124,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1514,7 +1514,7 @@
   <dimension ref="A1:CG22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="BS4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CC12" sqref="CC12"/>
+      <selection activeCell="CC6" sqref="CC6:CE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1543,380 +1543,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
-      <c r="AG1" s="78"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="78"/>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="78"/>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="78"/>
-      <c r="AU1" s="78"/>
-      <c r="AV1" s="78"/>
-      <c r="AW1" s="78"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="78"/>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="78"/>
-      <c r="BB1" s="78"/>
-      <c r="BC1" s="78"/>
-      <c r="BD1" s="78"/>
-      <c r="BE1" s="78"/>
-      <c r="BF1" s="78"/>
-      <c r="BG1" s="78"/>
-      <c r="BH1" s="78"/>
-      <c r="BI1" s="78"/>
-      <c r="BJ1" s="78"/>
-      <c r="BK1" s="78"/>
-      <c r="BL1" s="78"/>
-      <c r="BM1" s="78"/>
-      <c r="BN1" s="78"/>
-      <c r="BO1" s="78"/>
-      <c r="BP1" s="78"/>
-      <c r="BQ1" s="78"/>
-      <c r="BR1" s="79"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="72"/>
+      <c r="AF1" s="72"/>
+      <c r="AG1" s="72"/>
+      <c r="AH1" s="72"/>
+      <c r="AI1" s="72"/>
+      <c r="AJ1" s="72"/>
+      <c r="AK1" s="72"/>
+      <c r="AL1" s="72"/>
+      <c r="AM1" s="72"/>
+      <c r="AN1" s="72"/>
+      <c r="AO1" s="72"/>
+      <c r="AP1" s="72"/>
+      <c r="AQ1" s="72"/>
+      <c r="AR1" s="72"/>
+      <c r="AS1" s="72"/>
+      <c r="AT1" s="72"/>
+      <c r="AU1" s="72"/>
+      <c r="AV1" s="72"/>
+      <c r="AW1" s="72"/>
+      <c r="AX1" s="72"/>
+      <c r="AY1" s="72"/>
+      <c r="AZ1" s="72"/>
+      <c r="BA1" s="72"/>
+      <c r="BB1" s="72"/>
+      <c r="BC1" s="72"/>
+      <c r="BD1" s="72"/>
+      <c r="BE1" s="72"/>
+      <c r="BF1" s="72"/>
+      <c r="BG1" s="72"/>
+      <c r="BH1" s="72"/>
+      <c r="BI1" s="72"/>
+      <c r="BJ1" s="72"/>
+      <c r="BK1" s="72"/>
+      <c r="BL1" s="72"/>
+      <c r="BM1" s="72"/>
+      <c r="BN1" s="72"/>
+      <c r="BO1" s="72"/>
+      <c r="BP1" s="72"/>
+      <c r="BQ1" s="72"/>
+      <c r="BR1" s="73"/>
     </row>
     <row r="3" spans="1:85" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="80"/>
-      <c r="U3" s="80"/>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="80"/>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="80"/>
-      <c r="AC3" s="80"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="80"/>
-      <c r="AH3" s="80"/>
-      <c r="AI3" s="80"/>
-      <c r="AJ3" s="80"/>
-      <c r="AK3" s="80"/>
-      <c r="AL3" s="80"/>
-      <c r="AM3" s="80"/>
-      <c r="AN3" s="80"/>
-      <c r="AO3" s="80"/>
-      <c r="AP3" s="80"/>
-      <c r="AQ3" s="80"/>
-      <c r="AR3" s="80"/>
-      <c r="AS3" s="80"/>
-      <c r="AT3" s="80"/>
-      <c r="AU3" s="80"/>
-      <c r="AV3" s="80"/>
-      <c r="AW3" s="80"/>
-      <c r="AX3" s="80"/>
-      <c r="AY3" s="80"/>
-      <c r="AZ3" s="80"/>
-      <c r="BA3" s="80"/>
-      <c r="BB3" s="80"/>
-      <c r="BC3" s="80"/>
-      <c r="BD3" s="80"/>
-      <c r="BE3" s="80"/>
-      <c r="BF3" s="80"/>
-      <c r="BG3" s="80"/>
-      <c r="BH3" s="80"/>
-      <c r="BI3" s="80"/>
-      <c r="BJ3" s="80"/>
-      <c r="BK3" s="80"/>
-      <c r="BL3" s="80"/>
-      <c r="BM3" s="80"/>
-      <c r="BN3" s="80"/>
-      <c r="BO3" s="80"/>
-      <c r="BP3" s="80"/>
-      <c r="BQ3" s="80"/>
-      <c r="BR3" s="80"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
+      <c r="AC3" s="74"/>
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="74"/>
+      <c r="AF3" s="74"/>
+      <c r="AG3" s="74"/>
+      <c r="AH3" s="74"/>
+      <c r="AI3" s="74"/>
+      <c r="AJ3" s="74"/>
+      <c r="AK3" s="74"/>
+      <c r="AL3" s="74"/>
+      <c r="AM3" s="74"/>
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="74"/>
+      <c r="AP3" s="74"/>
+      <c r="AQ3" s="74"/>
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="74"/>
+      <c r="AT3" s="74"/>
+      <c r="AU3" s="74"/>
+      <c r="AV3" s="74"/>
+      <c r="AW3" s="74"/>
+      <c r="AX3" s="74"/>
+      <c r="AY3" s="74"/>
+      <c r="AZ3" s="74"/>
+      <c r="BA3" s="74"/>
+      <c r="BB3" s="74"/>
+      <c r="BC3" s="74"/>
+      <c r="BD3" s="74"/>
+      <c r="BE3" s="74"/>
+      <c r="BF3" s="74"/>
+      <c r="BG3" s="74"/>
+      <c r="BH3" s="74"/>
+      <c r="BI3" s="74"/>
+      <c r="BJ3" s="74"/>
+      <c r="BK3" s="74"/>
+      <c r="BL3" s="74"/>
+      <c r="BM3" s="74"/>
+      <c r="BN3" s="74"/>
+      <c r="BO3" s="74"/>
+      <c r="BP3" s="74"/>
+      <c r="BQ3" s="74"/>
+      <c r="BR3" s="74"/>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.45">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="82"/>
-      <c r="AE4" s="82"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="82"/>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="82"/>
-      <c r="AK4" s="82"/>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="82"/>
-      <c r="AO4" s="82"/>
-      <c r="AP4" s="82"/>
-      <c r="AQ4" s="82"/>
-      <c r="AR4" s="82"/>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="82"/>
-      <c r="AV4" s="82"/>
-      <c r="AW4" s="82"/>
-      <c r="AX4" s="82"/>
-      <c r="AY4" s="82"/>
-      <c r="AZ4" s="82"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="82"/>
-      <c r="BC4" s="82"/>
-      <c r="BD4" s="82"/>
-      <c r="BE4" s="82"/>
-      <c r="BF4" s="82"/>
-      <c r="BG4" s="82"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="82"/>
-      <c r="BJ4" s="82"/>
-      <c r="BK4" s="82"/>
-      <c r="BL4" s="82"/>
-      <c r="BM4" s="82"/>
-      <c r="BN4" s="82"/>
-      <c r="BO4" s="82"/>
-      <c r="BP4" s="82"/>
-      <c r="BQ4" s="82"/>
-      <c r="BR4" s="82"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="76"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="76"/>
+      <c r="BM4" s="76"/>
+      <c r="BN4" s="76"/>
+      <c r="BO4" s="76"/>
+      <c r="BP4" s="76"/>
+      <c r="BQ4" s="76"/>
+      <c r="BR4" s="76"/>
     </row>
     <row r="5" spans="1:85" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="6" spans="1:85" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="74" t="s">
+      <c r="D6" s="69"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="74" t="s">
+      <c r="G6" s="69"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="75"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="74" t="s">
+      <c r="J6" s="69"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="75"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="74" t="s">
+      <c r="M6" s="69"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="74" t="s">
+      <c r="P6" s="69"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="75"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="74" t="s">
+      <c r="S6" s="69"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="75"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="74" t="s">
+      <c r="V6" s="69"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="81"/>
-      <c r="AA6" s="74" t="s">
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="81"/>
-      <c r="AD6" s="74" t="s">
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="75"/>
+      <c r="AD6" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="AE6" s="75"/>
-      <c r="AF6" s="81"/>
-      <c r="AG6" s="74" t="s">
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="75"/>
+      <c r="AG6" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="75"/>
-      <c r="AI6" s="81"/>
-      <c r="AJ6" s="74" t="s">
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="75"/>
+      <c r="AJ6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AK6" s="75"/>
-      <c r="AL6" s="81"/>
-      <c r="AM6" s="74" t="s">
+      <c r="AK6" s="69"/>
+      <c r="AL6" s="75"/>
+      <c r="AM6" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="AN6" s="75"/>
-      <c r="AO6" s="76"/>
-      <c r="AP6" s="74" t="s">
+      <c r="AN6" s="69"/>
+      <c r="AO6" s="70"/>
+      <c r="AP6" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AQ6" s="75"/>
-      <c r="AR6" s="76"/>
-      <c r="AS6" s="74" t="s">
+      <c r="AQ6" s="69"/>
+      <c r="AR6" s="70"/>
+      <c r="AS6" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="75"/>
-      <c r="AU6" s="76"/>
-      <c r="AV6" s="74" t="s">
+      <c r="AT6" s="69"/>
+      <c r="AU6" s="70"/>
+      <c r="AV6" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AW6" s="75"/>
-      <c r="AX6" s="76"/>
-      <c r="AY6" s="74" t="s">
+      <c r="AW6" s="69"/>
+      <c r="AX6" s="70"/>
+      <c r="AY6" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="76"/>
-      <c r="BB6" s="74" t="s">
+      <c r="AZ6" s="69"/>
+      <c r="BA6" s="70"/>
+      <c r="BB6" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="75"/>
-      <c r="BD6" s="76"/>
-      <c r="BE6" s="74" t="s">
+      <c r="BC6" s="69"/>
+      <c r="BD6" s="70"/>
+      <c r="BE6" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="BF6" s="75"/>
-      <c r="BG6" s="76"/>
-      <c r="BH6" s="74" t="s">
+      <c r="BF6" s="69"/>
+      <c r="BG6" s="70"/>
+      <c r="BH6" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="BI6" s="75"/>
-      <c r="BJ6" s="76"/>
-      <c r="BK6" s="74" t="s">
+      <c r="BI6" s="69"/>
+      <c r="BJ6" s="70"/>
+      <c r="BK6" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="BL6" s="75"/>
-      <c r="BM6" s="76"/>
-      <c r="BN6" s="74" t="s">
+      <c r="BL6" s="69"/>
+      <c r="BM6" s="70"/>
+      <c r="BN6" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="BO6" s="75"/>
-      <c r="BP6" s="76"/>
-      <c r="BQ6" s="74" t="s">
+      <c r="BO6" s="69"/>
+      <c r="BP6" s="70"/>
+      <c r="BQ6" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="BR6" s="75"/>
-      <c r="BS6" s="76"/>
-      <c r="BT6" s="74" t="s">
+      <c r="BR6" s="69"/>
+      <c r="BS6" s="70"/>
+      <c r="BT6" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="BU6" s="75"/>
-      <c r="BV6" s="76"/>
-      <c r="BW6" s="74" t="s">
+      <c r="BU6" s="69"/>
+      <c r="BV6" s="70"/>
+      <c r="BW6" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="BX6" s="75"/>
-      <c r="BY6" s="76"/>
-      <c r="BZ6" s="74" t="s">
+      <c r="BX6" s="69"/>
+      <c r="BY6" s="70"/>
+      <c r="BZ6" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="CA6" s="75"/>
-      <c r="CB6" s="76"/>
-      <c r="CC6" s="74" t="s">
+      <c r="CA6" s="69"/>
+      <c r="CB6" s="70"/>
+      <c r="CC6" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="CD6" s="75"/>
-      <c r="CE6" s="76"/>
-      <c r="CF6" s="70" t="s">
+      <c r="CD6" s="69"/>
+      <c r="CE6" s="70"/>
+      <c r="CF6" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="CG6" s="72" t="s">
+      <c r="CG6" s="83" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:85" x14ac:dyDescent="0.45">
-      <c r="A7" s="84"/>
-      <c r="B7" s="69"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2160,8 +2160,8 @@
       <c r="CE7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CF7" s="71"/>
-      <c r="CG7" s="73"/>
+      <c r="CF7" s="82"/>
+      <c r="CG7" s="84"/>
     </row>
     <row r="8" spans="1:85" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="57"/>
@@ -2899,6 +2899,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="BH6:BJ6"/>
+    <mergeCell ref="BW6:BY6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="CF6:CF7"/>
+    <mergeCell ref="CG6:CG7"/>
+    <mergeCell ref="BT6:BV6"/>
+    <mergeCell ref="BN6:BP6"/>
+    <mergeCell ref="AM6:AO6"/>
+    <mergeCell ref="BQ6:BS6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="BK6:BM6"/>
+    <mergeCell ref="AS6:AU6"/>
+    <mergeCell ref="AV6:AX6"/>
+    <mergeCell ref="AY6:BA6"/>
+    <mergeCell ref="BB6:BD6"/>
+    <mergeCell ref="BE6:BG6"/>
     <mergeCell ref="BZ6:CB6"/>
     <mergeCell ref="CC6:CE6"/>
     <mergeCell ref="A1:BR1"/>
@@ -2915,24 +2933,6 @@
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="A4:BR4"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="CF6:CF7"/>
-    <mergeCell ref="CG6:CG7"/>
-    <mergeCell ref="BT6:BV6"/>
-    <mergeCell ref="BN6:BP6"/>
-    <mergeCell ref="AM6:AO6"/>
-    <mergeCell ref="BQ6:BS6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="BK6:BM6"/>
-    <mergeCell ref="AS6:AU6"/>
-    <mergeCell ref="AV6:AX6"/>
-    <mergeCell ref="AY6:BA6"/>
-    <mergeCell ref="BB6:BD6"/>
-    <mergeCell ref="BE6:BG6"/>
-    <mergeCell ref="BH6:BJ6"/>
-    <mergeCell ref="BW6:BY6"/>
   </mergeCells>
   <conditionalFormatting sqref="CF8:CF9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -2963,20 +2963,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="79"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="43"/>
@@ -3111,42 +3111,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
DebiCheck Tracking TSR update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9789CDBF-BB03-4C32-A480-4279C67D5038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F3AAD-70B4-4036-85F1-C9A3AB30563B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="76">
   <si>
     <t xml:space="preserve">Cancer </t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>Cancer R99</t>
+  </si>
+  <si>
+    <t>Higher Premium</t>
+  </si>
+  <si>
+    <t>Lower Premium</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -261,9 +270,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -902,9 +911,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -947,9 +956,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1059,14 +1068,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1075,6 +1084,8 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,23 +1095,32 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1108,23 +1128,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1144,13 +1155,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1513,110 +1524,110 @@
   </sheetPr>
   <dimension ref="A1:CG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BS4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="BS4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="CC6" sqref="CC6:CE6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.3984375" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" customWidth="1"/>
-    <col min="3" max="20" width="10.265625" style="3" customWidth="1"/>
-    <col min="21" max="41" width="10.265625" customWidth="1"/>
-    <col min="42" max="42" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="20" width="10.28515625" style="3" customWidth="1"/>
+    <col min="21" max="41" width="10.28515625" customWidth="1"/>
+    <col min="42" max="42" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="10" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="10" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="10" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.73046875" customWidth="1"/>
+    <col min="70" max="70" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:85" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
-      <c r="AK1" s="72"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="72"/>
-      <c r="AN1" s="72"/>
-      <c r="AO1" s="72"/>
-      <c r="AP1" s="72"/>
-      <c r="AQ1" s="72"/>
-      <c r="AR1" s="72"/>
-      <c r="AS1" s="72"/>
-      <c r="AT1" s="72"/>
-      <c r="AU1" s="72"/>
-      <c r="AV1" s="72"/>
-      <c r="AW1" s="72"/>
-      <c r="AX1" s="72"/>
-      <c r="AY1" s="72"/>
-      <c r="AZ1" s="72"/>
-      <c r="BA1" s="72"/>
-      <c r="BB1" s="72"/>
-      <c r="BC1" s="72"/>
-      <c r="BD1" s="72"/>
-      <c r="BE1" s="72"/>
-      <c r="BF1" s="72"/>
-      <c r="BG1" s="72"/>
-      <c r="BH1" s="72"/>
-      <c r="BI1" s="72"/>
-      <c r="BJ1" s="72"/>
-      <c r="BK1" s="72"/>
-      <c r="BL1" s="72"/>
-      <c r="BM1" s="72"/>
-      <c r="BN1" s="72"/>
-      <c r="BO1" s="72"/>
-      <c r="BP1" s="72"/>
-      <c r="BQ1" s="72"/>
-      <c r="BR1" s="73"/>
-    </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.45">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+      <c r="AA1" s="85"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="85"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="85"/>
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="85"/>
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="85"/>
+      <c r="AM1" s="85"/>
+      <c r="AN1" s="85"/>
+      <c r="AO1" s="85"/>
+      <c r="AP1" s="85"/>
+      <c r="AQ1" s="85"/>
+      <c r="AR1" s="85"/>
+      <c r="AS1" s="85"/>
+      <c r="AT1" s="85"/>
+      <c r="AU1" s="85"/>
+      <c r="AV1" s="85"/>
+      <c r="AW1" s="85"/>
+      <c r="AX1" s="85"/>
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="85"/>
+      <c r="BA1" s="85"/>
+      <c r="BB1" s="85"/>
+      <c r="BC1" s="85"/>
+      <c r="BD1" s="85"/>
+      <c r="BE1" s="85"/>
+      <c r="BF1" s="85"/>
+      <c r="BG1" s="85"/>
+      <c r="BH1" s="85"/>
+      <c r="BI1" s="85"/>
+      <c r="BJ1" s="85"/>
+      <c r="BK1" s="85"/>
+      <c r="BL1" s="85"/>
+      <c r="BM1" s="85"/>
+      <c r="BN1" s="85"/>
+      <c r="BO1" s="85"/>
+      <c r="BP1" s="85"/>
+      <c r="BQ1" s="85"/>
+      <c r="BR1" s="86"/>
+    </row>
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
@@ -1690,233 +1701,233 @@
       <c r="BQ3" s="74"/>
       <c r="BR3" s="74"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="76"/>
-      <c r="AH4" s="76"/>
-      <c r="AI4" s="76"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
-      <c r="AN4" s="76"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="76"/>
-      <c r="AT4" s="76"/>
-      <c r="AU4" s="76"/>
-      <c r="AV4" s="76"/>
-      <c r="AW4" s="76"/>
-      <c r="AX4" s="76"/>
-      <c r="AY4" s="76"/>
-      <c r="AZ4" s="76"/>
-      <c r="BA4" s="76"/>
-      <c r="BB4" s="76"/>
-      <c r="BC4" s="76"/>
-      <c r="BD4" s="76"/>
-      <c r="BE4" s="76"/>
-      <c r="BF4" s="76"/>
-      <c r="BG4" s="76"/>
-      <c r="BH4" s="76"/>
-      <c r="BI4" s="76"/>
-      <c r="BJ4" s="76"/>
-      <c r="BK4" s="76"/>
-      <c r="BL4" s="76"/>
-      <c r="BM4" s="76"/>
-      <c r="BN4" s="76"/>
-      <c r="BO4" s="76"/>
-      <c r="BP4" s="76"/>
-      <c r="BQ4" s="76"/>
-      <c r="BR4" s="76"/>
-    </row>
-    <row r="5" spans="1:85" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:85" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="77" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="75"/>
+      <c r="AF4" s="75"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="75"/>
+      <c r="AL4" s="75"/>
+      <c r="AM4" s="75"/>
+      <c r="AN4" s="75"/>
+      <c r="AO4" s="75"/>
+      <c r="AP4" s="75"/>
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="75"/>
+      <c r="AS4" s="75"/>
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="75"/>
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="75"/>
+      <c r="BN4" s="75"/>
+      <c r="BO4" s="75"/>
+      <c r="BP4" s="75"/>
+      <c r="BQ4" s="75"/>
+      <c r="BR4" s="75"/>
+    </row>
+    <row r="5" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="68" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="68" t="s">
+      <c r="G6" s="71"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="69"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="68" t="s">
+      <c r="J6" s="71"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="69"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="68" t="s">
+      <c r="M6" s="71"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="68" t="s">
+      <c r="P6" s="71"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="69"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="68" t="s">
+      <c r="S6" s="71"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="69"/>
-      <c r="W6" s="75"/>
-      <c r="X6" s="68" t="s">
+      <c r="V6" s="71"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="75"/>
-      <c r="AA6" s="68" t="s">
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="73"/>
+      <c r="AA6" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="68" t="s">
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="73"/>
+      <c r="AD6" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="75"/>
-      <c r="AG6" s="68" t="s">
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="73"/>
+      <c r="AG6" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="69"/>
-      <c r="AI6" s="75"/>
-      <c r="AJ6" s="68" t="s">
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="73"/>
+      <c r="AJ6" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="75"/>
-      <c r="AM6" s="68" t="s">
+      <c r="AK6" s="71"/>
+      <c r="AL6" s="73"/>
+      <c r="AM6" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="AN6" s="69"/>
-      <c r="AO6" s="70"/>
-      <c r="AP6" s="68" t="s">
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="72"/>
+      <c r="AP6" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="AQ6" s="69"/>
-      <c r="AR6" s="70"/>
-      <c r="AS6" s="68" t="s">
+      <c r="AQ6" s="71"/>
+      <c r="AR6" s="72"/>
+      <c r="AS6" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="69"/>
-      <c r="AU6" s="70"/>
-      <c r="AV6" s="68" t="s">
+      <c r="AT6" s="71"/>
+      <c r="AU6" s="72"/>
+      <c r="AV6" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="70"/>
-      <c r="AY6" s="68" t="s">
+      <c r="AW6" s="71"/>
+      <c r="AX6" s="72"/>
+      <c r="AY6" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="AZ6" s="69"/>
-      <c r="BA6" s="70"/>
-      <c r="BB6" s="68" t="s">
+      <c r="AZ6" s="71"/>
+      <c r="BA6" s="72"/>
+      <c r="BB6" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="69"/>
-      <c r="BD6" s="70"/>
-      <c r="BE6" s="68" t="s">
+      <c r="BC6" s="71"/>
+      <c r="BD6" s="72"/>
+      <c r="BE6" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="BF6" s="69"/>
-      <c r="BG6" s="70"/>
-      <c r="BH6" s="68" t="s">
+      <c r="BF6" s="71"/>
+      <c r="BG6" s="72"/>
+      <c r="BH6" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="BI6" s="69"/>
-      <c r="BJ6" s="70"/>
-      <c r="BK6" s="68" t="s">
+      <c r="BI6" s="71"/>
+      <c r="BJ6" s="72"/>
+      <c r="BK6" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="BL6" s="69"/>
-      <c r="BM6" s="70"/>
-      <c r="BN6" s="68" t="s">
+      <c r="BL6" s="71"/>
+      <c r="BM6" s="72"/>
+      <c r="BN6" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="BO6" s="69"/>
-      <c r="BP6" s="70"/>
-      <c r="BQ6" s="68" t="s">
+      <c r="BO6" s="71"/>
+      <c r="BP6" s="72"/>
+      <c r="BQ6" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="BR6" s="69"/>
-      <c r="BS6" s="70"/>
-      <c r="BT6" s="68" t="s">
+      <c r="BR6" s="71"/>
+      <c r="BS6" s="72"/>
+      <c r="BT6" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="BU6" s="69"/>
-      <c r="BV6" s="70"/>
-      <c r="BW6" s="68" t="s">
+      <c r="BU6" s="71"/>
+      <c r="BV6" s="72"/>
+      <c r="BW6" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="BX6" s="69"/>
-      <c r="BY6" s="70"/>
-      <c r="BZ6" s="68" t="s">
+      <c r="BX6" s="71"/>
+      <c r="BY6" s="72"/>
+      <c r="BZ6" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="CA6" s="69"/>
-      <c r="CB6" s="70"/>
-      <c r="CC6" s="68" t="s">
+      <c r="CA6" s="71"/>
+      <c r="CB6" s="72"/>
+      <c r="CC6" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="CD6" s="69"/>
-      <c r="CE6" s="70"/>
-      <c r="CF6" s="81" t="s">
+      <c r="CD6" s="71"/>
+      <c r="CE6" s="72"/>
+      <c r="CF6" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="CG6" s="83" t="s">
+      <c r="CG6" s="80" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.45">
-      <c r="A7" s="78"/>
-      <c r="B7" s="80"/>
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A7" s="83"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2160,10 +2171,10 @@
       <c r="CE7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CF7" s="82"/>
-      <c r="CG7" s="84"/>
-    </row>
-    <row r="8" spans="1:85" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="CF7" s="79"/>
+      <c r="CG7" s="81"/>
+    </row>
+    <row r="8" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
       <c r="B8" s="58"/>
       <c r="C8" s="33"/>
@@ -2250,7 +2261,7 @@
       <c r="CF8" s="55"/>
       <c r="CG8" s="45"/>
     </row>
-    <row r="9" spans="1:85" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:85" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
@@ -2338,7 +2349,7 @@
       <c r="CE9" s="30"/>
       <c r="CF9" s="56"/>
     </row>
-    <row r="10" spans="1:85" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="39"/>
@@ -2381,7 +2392,7 @@
       <c r="AN10" s="38"/>
       <c r="AO10" s="38"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="39"/>
@@ -2424,7 +2435,7 @@
       <c r="AN11" s="39"/>
       <c r="AO11" s="38"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="39"/>
@@ -2467,7 +2478,7 @@
       <c r="AN12" s="38"/>
       <c r="AO12" s="38"/>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="39"/>
@@ -2510,7 +2521,7 @@
       <c r="AN13" s="38"/>
       <c r="AO13" s="38"/>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="39"/>
@@ -2553,7 +2564,7 @@
       <c r="AN14" s="38"/>
       <c r="AO14" s="38"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="39"/>
@@ -2596,7 +2607,7 @@
       <c r="AN15" s="38"/>
       <c r="AO15" s="38"/>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="39"/>
@@ -2639,7 +2650,7 @@
       <c r="AN16" s="38"/>
       <c r="AO16" s="38"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="39"/>
@@ -2682,7 +2693,7 @@
       <c r="AN17" s="38"/>
       <c r="AO17" s="38"/>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="39"/>
@@ -2725,7 +2736,7 @@
       <c r="AN18" s="38"/>
       <c r="AO18" s="38"/>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="39"/>
@@ -2768,7 +2779,7 @@
       <c r="AN19" s="38"/>
       <c r="AO19" s="38"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="39"/>
@@ -2811,7 +2822,7 @@
       <c r="AN20" s="38"/>
       <c r="AO20" s="38"/>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="39"/>
@@ -2854,7 +2865,7 @@
       <c r="AN21" s="38"/>
       <c r="AO21" s="38"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="39"/>
@@ -2899,11 +2910,18 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="BH6:BJ6"/>
-    <mergeCell ref="BW6:BY6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A1:BR1"/>
+    <mergeCell ref="A3:BR3"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="AJ6:AL6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="CF6:CF7"/>
     <mergeCell ref="CG6:CG7"/>
     <mergeCell ref="BT6:BV6"/>
@@ -2917,22 +2935,15 @@
     <mergeCell ref="AY6:BA6"/>
     <mergeCell ref="BB6:BD6"/>
     <mergeCell ref="BE6:BG6"/>
+    <mergeCell ref="BH6:BJ6"/>
+    <mergeCell ref="BW6:BY6"/>
     <mergeCell ref="BZ6:CB6"/>
     <mergeCell ref="CC6:CE6"/>
-    <mergeCell ref="A1:BR1"/>
-    <mergeCell ref="A3:BR3"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="AJ6:AL6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="A4:BR4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="CF8:CF9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -2949,42 +2960,53 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="3" width="24.1328125" customWidth="1"/>
-    <col min="4" max="4" width="26.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="74"/>
       <c r="C3" s="74"/>
       <c r="D3" s="74"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="C4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>18</v>
       </c>
@@ -2997,89 +3019,105 @@
       <c r="D6" s="50" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E6" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="47"/>
       <c r="C7" s="27"/>
       <c r="D7" s="53"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="39"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3097,39 +3135,39 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1328125" customWidth="1"/>
-    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11.3984375" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="73"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="86"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>40</v>
       </c>
@@ -3148,31 +3186,31 @@
       <c r="N3" s="74"/>
       <c r="O3" s="74"/>
     </row>
-    <row r="4" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="85" t="s">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="85" t="s">
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="86"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="85" t="s">
+      <c r="J5" s="88"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="87"/>
-    </row>
-    <row r="6" spans="1:15" s="16" customFormat="1" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="89"/>
+    </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
@@ -3219,7 +3257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="13"/>
       <c r="C7" s="42"/>
@@ -3236,8 +3274,8 @@
       <c r="N7" s="18"/>
       <c r="O7" s="19"/>
     </row>
-    <row r="8" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3284,10 +3322,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10" s="15"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="15"/>
     </row>
   </sheetData>
@@ -3309,84 +3347,84 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.3984375" customWidth="1"/>
-    <col min="2" max="19" width="11.265625" style="3" customWidth="1"/>
-    <col min="20" max="37" width="11.265625" customWidth="1"/>
-    <col min="38" max="38" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="19" width="11.28515625" style="3" customWidth="1"/>
+    <col min="20" max="37" width="11.28515625" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89" t="s">
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89" t="s">
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89" t="s">
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89" t="s">
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89" t="s">
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89" t="s">
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89" t="s">
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89" t="s">
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="89" t="s">
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="89"/>
-      <c r="AL1" s="89" t="s">
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3537,14 +3575,14 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
-    <col min="2" max="2" width="30.265625" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -3569,35 +3607,35 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" style="63" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" style="63" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" style="63" customWidth="1"/>
-    <col min="6" max="6" width="14.73046875" style="63" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="63" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="63" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="63" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C5" s="91" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="93"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="95"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>18</v>
       </c>
@@ -3617,7 +3655,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="65"/>

</xml_diff>

<commit_message>
Temp Salary Report Update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F3AAD-70B4-4036-85F1-C9A3AB30563B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5F15C0-D572-437D-8FD7-A501ED3A22A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="79">
   <si>
     <t xml:space="preserve">Cancer </t>
   </si>
@@ -263,6 +263,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>DebiCheck Incentive</t>
+  </si>
+  <si>
+    <t>Total DebiCheck Incentive</t>
+  </si>
+  <si>
+    <t>DebiCheck</t>
   </si>
 </sst>
 </file>
@@ -270,9 +279,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -911,9 +920,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -956,9 +965,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,14 +1077,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1086,19 +1095,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1110,33 +1140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1152,17 +1161,20 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1554,380 +1566,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="85"/>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
-      <c r="AM1" s="85"/>
-      <c r="AN1" s="85"/>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="85"/>
-      <c r="AR1" s="85"/>
-      <c r="AS1" s="85"/>
-      <c r="AT1" s="85"/>
-      <c r="AU1" s="85"/>
-      <c r="AV1" s="85"/>
-      <c r="AW1" s="85"/>
-      <c r="AX1" s="85"/>
-      <c r="AY1" s="85"/>
-      <c r="AZ1" s="85"/>
-      <c r="BA1" s="85"/>
-      <c r="BB1" s="85"/>
-      <c r="BC1" s="85"/>
-      <c r="BD1" s="85"/>
-      <c r="BE1" s="85"/>
-      <c r="BF1" s="85"/>
-      <c r="BG1" s="85"/>
-      <c r="BH1" s="85"/>
-      <c r="BI1" s="85"/>
-      <c r="BJ1" s="85"/>
-      <c r="BK1" s="85"/>
-      <c r="BL1" s="85"/>
-      <c r="BM1" s="85"/>
-      <c r="BN1" s="85"/>
-      <c r="BO1" s="85"/>
-      <c r="BP1" s="85"/>
-      <c r="BQ1" s="85"/>
-      <c r="BR1" s="86"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="71"/>
+      <c r="AP1" s="71"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="71"/>
+      <c r="AU1" s="71"/>
+      <c r="AV1" s="71"/>
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="71"/>
+      <c r="AY1" s="71"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="71"/>
+      <c r="BB1" s="71"/>
+      <c r="BC1" s="71"/>
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="71"/>
+      <c r="BH1" s="71"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="71"/>
+      <c r="BK1" s="71"/>
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="71"/>
+      <c r="BN1" s="71"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="71"/>
+      <c r="BQ1" s="71"/>
+      <c r="BR1" s="72"/>
     </row>
     <row r="3" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="74"/>
-      <c r="AF3" s="74"/>
-      <c r="AG3" s="74"/>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="74"/>
-      <c r="AJ3" s="74"/>
-      <c r="AK3" s="74"/>
-      <c r="AL3" s="74"/>
-      <c r="AM3" s="74"/>
-      <c r="AN3" s="74"/>
-      <c r="AO3" s="74"/>
-      <c r="AP3" s="74"/>
-      <c r="AQ3" s="74"/>
-      <c r="AR3" s="74"/>
-      <c r="AS3" s="74"/>
-      <c r="AT3" s="74"/>
-      <c r="AU3" s="74"/>
-      <c r="AV3" s="74"/>
-      <c r="AW3" s="74"/>
-      <c r="AX3" s="74"/>
-      <c r="AY3" s="74"/>
-      <c r="AZ3" s="74"/>
-      <c r="BA3" s="74"/>
-      <c r="BB3" s="74"/>
-      <c r="BC3" s="74"/>
-      <c r="BD3" s="74"/>
-      <c r="BE3" s="74"/>
-      <c r="BF3" s="74"/>
-      <c r="BG3" s="74"/>
-      <c r="BH3" s="74"/>
-      <c r="BI3" s="74"/>
-      <c r="BJ3" s="74"/>
-      <c r="BK3" s="74"/>
-      <c r="BL3" s="74"/>
-      <c r="BM3" s="74"/>
-      <c r="BN3" s="74"/>
-      <c r="BO3" s="74"/>
-      <c r="BP3" s="74"/>
-      <c r="BQ3" s="74"/>
-      <c r="BR3" s="74"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73"/>
+      <c r="AB3" s="73"/>
+      <c r="AC3" s="73"/>
+      <c r="AD3" s="73"/>
+      <c r="AE3" s="73"/>
+      <c r="AF3" s="73"/>
+      <c r="AG3" s="73"/>
+      <c r="AH3" s="73"/>
+      <c r="AI3" s="73"/>
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="73"/>
+      <c r="AL3" s="73"/>
+      <c r="AM3" s="73"/>
+      <c r="AN3" s="73"/>
+      <c r="AO3" s="73"/>
+      <c r="AP3" s="73"/>
+      <c r="AQ3" s="73"/>
+      <c r="AR3" s="73"/>
+      <c r="AS3" s="73"/>
+      <c r="AT3" s="73"/>
+      <c r="AU3" s="73"/>
+      <c r="AV3" s="73"/>
+      <c r="AW3" s="73"/>
+      <c r="AX3" s="73"/>
+      <c r="AY3" s="73"/>
+      <c r="AZ3" s="73"/>
+      <c r="BA3" s="73"/>
+      <c r="BB3" s="73"/>
+      <c r="BC3" s="73"/>
+      <c r="BD3" s="73"/>
+      <c r="BE3" s="73"/>
+      <c r="BF3" s="73"/>
+      <c r="BG3" s="73"/>
+      <c r="BH3" s="73"/>
+      <c r="BI3" s="73"/>
+      <c r="BJ3" s="73"/>
+      <c r="BK3" s="73"/>
+      <c r="BL3" s="73"/>
+      <c r="BM3" s="73"/>
+      <c r="BN3" s="73"/>
+      <c r="BO3" s="73"/>
+      <c r="BP3" s="73"/>
+      <c r="BQ3" s="73"/>
+      <c r="BR3" s="73"/>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="75"/>
-      <c r="AD4" s="75"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75"/>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="75"/>
-      <c r="AP4" s="75"/>
-      <c r="AQ4" s="75"/>
-      <c r="AR4" s="75"/>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="75"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="75"/>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="75"/>
-      <c r="BI4" s="75"/>
-      <c r="BJ4" s="75"/>
-      <c r="BK4" s="75"/>
-      <c r="BL4" s="75"/>
-      <c r="BM4" s="75"/>
-      <c r="BN4" s="75"/>
-      <c r="BO4" s="75"/>
-      <c r="BP4" s="75"/>
-      <c r="BQ4" s="75"/>
-      <c r="BR4" s="75"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="82"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="82"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="82"/>
+      <c r="AE4" s="82"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="82"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="82"/>
+      <c r="AJ4" s="82"/>
+      <c r="AK4" s="82"/>
+      <c r="AL4" s="82"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="82"/>
+      <c r="AO4" s="82"/>
+      <c r="AP4" s="82"/>
+      <c r="AQ4" s="82"/>
+      <c r="AR4" s="82"/>
+      <c r="AS4" s="82"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="82"/>
+      <c r="AV4" s="82"/>
+      <c r="AW4" s="82"/>
+      <c r="AX4" s="82"/>
+      <c r="AY4" s="82"/>
+      <c r="AZ4" s="82"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="82"/>
+      <c r="BC4" s="82"/>
+      <c r="BD4" s="82"/>
+      <c r="BE4" s="82"/>
+      <c r="BF4" s="82"/>
+      <c r="BG4" s="82"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="82"/>
+      <c r="BJ4" s="82"/>
+      <c r="BK4" s="82"/>
+      <c r="BL4" s="82"/>
+      <c r="BM4" s="82"/>
+      <c r="BN4" s="82"/>
+      <c r="BO4" s="82"/>
+      <c r="BP4" s="82"/>
+      <c r="BQ4" s="82"/>
+      <c r="BR4" s="82"/>
     </row>
     <row r="5" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="70" t="s">
+      <c r="D6" s="75"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="70" t="s">
+      <c r="G6" s="75"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="70" t="s">
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="70" t="s">
+      <c r="M6" s="75"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="70" t="s">
+      <c r="P6" s="75"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="71"/>
-      <c r="T6" s="73"/>
-      <c r="U6" s="70" t="s">
+      <c r="S6" s="75"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="71"/>
-      <c r="W6" s="73"/>
-      <c r="X6" s="70" t="s">
+      <c r="V6" s="75"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="71"/>
-      <c r="Z6" s="73"/>
-      <c r="AA6" s="70" t="s">
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="71"/>
-      <c r="AC6" s="73"/>
-      <c r="AD6" s="70" t="s">
+      <c r="AB6" s="75"/>
+      <c r="AC6" s="76"/>
+      <c r="AD6" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="AE6" s="71"/>
-      <c r="AF6" s="73"/>
-      <c r="AG6" s="70" t="s">
+      <c r="AE6" s="75"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="71"/>
-      <c r="AI6" s="73"/>
-      <c r="AJ6" s="70" t="s">
+      <c r="AH6" s="75"/>
+      <c r="AI6" s="76"/>
+      <c r="AJ6" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="AK6" s="71"/>
-      <c r="AL6" s="73"/>
-      <c r="AM6" s="70" t="s">
+      <c r="AK6" s="75"/>
+      <c r="AL6" s="76"/>
+      <c r="AM6" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="AN6" s="71"/>
-      <c r="AO6" s="72"/>
-      <c r="AP6" s="70" t="s">
+      <c r="AN6" s="75"/>
+      <c r="AO6" s="81"/>
+      <c r="AP6" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="AQ6" s="71"/>
-      <c r="AR6" s="72"/>
-      <c r="AS6" s="70" t="s">
+      <c r="AQ6" s="75"/>
+      <c r="AR6" s="81"/>
+      <c r="AS6" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="71"/>
-      <c r="AU6" s="72"/>
-      <c r="AV6" s="70" t="s">
+      <c r="AT6" s="75"/>
+      <c r="AU6" s="81"/>
+      <c r="AV6" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="AW6" s="71"/>
-      <c r="AX6" s="72"/>
-      <c r="AY6" s="70" t="s">
+      <c r="AW6" s="75"/>
+      <c r="AX6" s="81"/>
+      <c r="AY6" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="AZ6" s="71"/>
-      <c r="BA6" s="72"/>
-      <c r="BB6" s="70" t="s">
+      <c r="AZ6" s="75"/>
+      <c r="BA6" s="81"/>
+      <c r="BB6" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="71"/>
-      <c r="BD6" s="72"/>
-      <c r="BE6" s="70" t="s">
+      <c r="BC6" s="75"/>
+      <c r="BD6" s="81"/>
+      <c r="BE6" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="BF6" s="71"/>
-      <c r="BG6" s="72"/>
-      <c r="BH6" s="70" t="s">
+      <c r="BF6" s="75"/>
+      <c r="BG6" s="81"/>
+      <c r="BH6" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="BI6" s="71"/>
-      <c r="BJ6" s="72"/>
-      <c r="BK6" s="70" t="s">
+      <c r="BI6" s="75"/>
+      <c r="BJ6" s="81"/>
+      <c r="BK6" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="BL6" s="71"/>
-      <c r="BM6" s="72"/>
-      <c r="BN6" s="70" t="s">
+      <c r="BL6" s="75"/>
+      <c r="BM6" s="81"/>
+      <c r="BN6" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="BO6" s="71"/>
-      <c r="BP6" s="72"/>
-      <c r="BQ6" s="70" t="s">
+      <c r="BO6" s="75"/>
+      <c r="BP6" s="81"/>
+      <c r="BQ6" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="BR6" s="71"/>
-      <c r="BS6" s="72"/>
-      <c r="BT6" s="70" t="s">
+      <c r="BR6" s="75"/>
+      <c r="BS6" s="81"/>
+      <c r="BT6" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="BU6" s="71"/>
-      <c r="BV6" s="72"/>
-      <c r="BW6" s="70" t="s">
+      <c r="BU6" s="75"/>
+      <c r="BV6" s="81"/>
+      <c r="BW6" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="BX6" s="71"/>
-      <c r="BY6" s="72"/>
-      <c r="BZ6" s="70" t="s">
+      <c r="BX6" s="75"/>
+      <c r="BY6" s="81"/>
+      <c r="BZ6" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="CA6" s="71"/>
-      <c r="CB6" s="72"/>
-      <c r="CC6" s="70" t="s">
+      <c r="CA6" s="75"/>
+      <c r="CB6" s="81"/>
+      <c r="CC6" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="CD6" s="71"/>
-      <c r="CE6" s="72"/>
-      <c r="CF6" s="78" t="s">
+      <c r="CD6" s="75"/>
+      <c r="CE6" s="81"/>
+      <c r="CF6" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="CG6" s="80" t="s">
+      <c r="CG6" s="79" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="77"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2171,8 +2183,8 @@
       <c r="CE7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CF7" s="79"/>
-      <c r="CG7" s="81"/>
+      <c r="CF7" s="78"/>
+      <c r="CG7" s="80"/>
     </row>
     <row r="8" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
@@ -2910,18 +2922,12 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:BR1"/>
-    <mergeCell ref="A3:BR3"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="AJ6:AL6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="CC6:CE6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="A4:BR4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="CF6:CF7"/>
     <mergeCell ref="CG6:CG7"/>
     <mergeCell ref="BT6:BV6"/>
@@ -2938,12 +2944,18 @@
     <mergeCell ref="BH6:BJ6"/>
     <mergeCell ref="BW6:BY6"/>
     <mergeCell ref="BZ6:CB6"/>
-    <mergeCell ref="CC6:CE6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="A4:BR4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:BR1"/>
+    <mergeCell ref="A3:BR3"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="AJ6:AL6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O6:Q6"/>
   </mergeCells>
   <conditionalFormatting sqref="CF8:CF9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -2960,10 +2972,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,37 +2988,37 @@
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="86"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="72"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="C4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>18</v>
       </c>
@@ -3031,8 +3043,11 @@
       <c r="H6" s="69" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="69" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="47"/>
       <c r="C7" s="27"/>
@@ -3041,50 +3056,51 @@
       <c r="F7" s="68"/>
       <c r="G7" s="68"/>
       <c r="H7" s="68"/>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="68"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="39"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -3149,42 +3165,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="86"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3601,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61B72FE-9BBD-48F6-9138-132EDBC73A96}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,27 +3631,30 @@
     <col min="4" max="4" width="11.5703125" style="63" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="63" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="63" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="93" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>18</v>
       </c>
@@ -3654,19 +3673,36 @@
       <c r="F6" s="62" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="65"/>
       <c r="D7" s="65"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dane Temp Salary Report Update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dane Burts\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5F15C0-D572-437D-8FD7-A501ED3A22A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B28C00C-983D-4D25-9C2E-0C275E977641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
     <sheet name="Upgrades" sheetId="5" r:id="rId2"/>
-    <sheet name="Details" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Details" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet name="Final Incentive Summary" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t xml:space="preserve">Cancer </t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>DebiCheck</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Cancer Spouse</t>
   </si>
 </sst>
 </file>
@@ -279,9 +285,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -340,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -910,6 +916,26 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -920,9 +946,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -965,9 +991,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1077,14 +1103,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1095,6 +1121,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1115,6 +1162,12 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1134,18 +1187,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1158,23 +1208,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1534,837 +1583,866 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CG22"/>
+  <dimension ref="A1:CK22"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="BS4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CC6" sqref="CC6:CE6"/>
+    <sheetView view="pageLayout" topLeftCell="BL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BX6" sqref="BX6:BZ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="20" width="10.28515625" style="3" customWidth="1"/>
-    <col min="21" max="41" width="10.28515625" customWidth="1"/>
-    <col min="42" max="42" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="21" width="10.28515625" style="3" customWidth="1"/>
+    <col min="22" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:89" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
-      <c r="AB1" s="71"/>
-      <c r="AC1" s="71"/>
-      <c r="AD1" s="71"/>
-      <c r="AE1" s="71"/>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="71"/>
-      <c r="AH1" s="71"/>
-      <c r="AI1" s="71"/>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="71"/>
-      <c r="AM1" s="71"/>
-      <c r="AN1" s="71"/>
-      <c r="AO1" s="71"/>
-      <c r="AP1" s="71"/>
-      <c r="AQ1" s="71"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="71"/>
-      <c r="AT1" s="71"/>
-      <c r="AU1" s="71"/>
-      <c r="AV1" s="71"/>
-      <c r="AW1" s="71"/>
-      <c r="AX1" s="71"/>
-      <c r="AY1" s="71"/>
-      <c r="AZ1" s="71"/>
-      <c r="BA1" s="71"/>
-      <c r="BB1" s="71"/>
-      <c r="BC1" s="71"/>
-      <c r="BD1" s="71"/>
-      <c r="BE1" s="71"/>
-      <c r="BF1" s="71"/>
-      <c r="BG1" s="71"/>
-      <c r="BH1" s="71"/>
-      <c r="BI1" s="71"/>
-      <c r="BJ1" s="71"/>
-      <c r="BK1" s="71"/>
-      <c r="BL1" s="71"/>
-      <c r="BM1" s="71"/>
-      <c r="BN1" s="71"/>
-      <c r="BO1" s="71"/>
-      <c r="BP1" s="71"/>
-      <c r="BQ1" s="71"/>
-      <c r="BR1" s="72"/>
-    </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
+      <c r="BC1" s="78"/>
+      <c r="BD1" s="78"/>
+      <c r="BE1" s="78"/>
+      <c r="BF1" s="78"/>
+      <c r="BG1" s="78"/>
+      <c r="BH1" s="78"/>
+      <c r="BI1" s="78"/>
+      <c r="BJ1" s="78"/>
+      <c r="BK1" s="78"/>
+      <c r="BL1" s="78"/>
+      <c r="BM1" s="78"/>
+      <c r="BN1" s="78"/>
+      <c r="BO1" s="78"/>
+      <c r="BP1" s="78"/>
+      <c r="BQ1" s="78"/>
+      <c r="BR1" s="78"/>
+      <c r="BS1" s="79"/>
+    </row>
+    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="73"/>
-      <c r="AC3" s="73"/>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="73"/>
-      <c r="AI3" s="73"/>
-      <c r="AJ3" s="73"/>
-      <c r="AK3" s="73"/>
-      <c r="AL3" s="73"/>
-      <c r="AM3" s="73"/>
-      <c r="AN3" s="73"/>
-      <c r="AO3" s="73"/>
-      <c r="AP3" s="73"/>
-      <c r="AQ3" s="73"/>
-      <c r="AR3" s="73"/>
-      <c r="AS3" s="73"/>
-      <c r="AT3" s="73"/>
-      <c r="AU3" s="73"/>
-      <c r="AV3" s="73"/>
-      <c r="AW3" s="73"/>
-      <c r="AX3" s="73"/>
-      <c r="AY3" s="73"/>
-      <c r="AZ3" s="73"/>
-      <c r="BA3" s="73"/>
-      <c r="BB3" s="73"/>
-      <c r="BC3" s="73"/>
-      <c r="BD3" s="73"/>
-      <c r="BE3" s="73"/>
-      <c r="BF3" s="73"/>
-      <c r="BG3" s="73"/>
-      <c r="BH3" s="73"/>
-      <c r="BI3" s="73"/>
-      <c r="BJ3" s="73"/>
-      <c r="BK3" s="73"/>
-      <c r="BL3" s="73"/>
-      <c r="BM3" s="73"/>
-      <c r="BN3" s="73"/>
-      <c r="BO3" s="73"/>
-      <c r="BP3" s="73"/>
-      <c r="BQ3" s="73"/>
-      <c r="BR3" s="73"/>
-    </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
+      <c r="AA3" s="80"/>
+      <c r="AB3" s="80"/>
+      <c r="AC3" s="80"/>
+      <c r="AD3" s="80"/>
+      <c r="AE3" s="80"/>
+      <c r="AF3" s="80"/>
+      <c r="AG3" s="80"/>
+      <c r="AH3" s="80"/>
+      <c r="AI3" s="80"/>
+      <c r="AJ3" s="80"/>
+      <c r="AK3" s="80"/>
+      <c r="AL3" s="80"/>
+      <c r="AM3" s="80"/>
+      <c r="AN3" s="80"/>
+      <c r="AO3" s="80"/>
+      <c r="AP3" s="80"/>
+      <c r="AQ3" s="80"/>
+      <c r="AR3" s="80"/>
+      <c r="AS3" s="80"/>
+      <c r="AT3" s="80"/>
+      <c r="AU3" s="80"/>
+      <c r="AV3" s="80"/>
+      <c r="AW3" s="80"/>
+      <c r="AX3" s="80"/>
+      <c r="AY3" s="80"/>
+      <c r="AZ3" s="80"/>
+      <c r="BA3" s="80"/>
+      <c r="BB3" s="80"/>
+      <c r="BC3" s="80"/>
+      <c r="BD3" s="80"/>
+      <c r="BE3" s="80"/>
+      <c r="BF3" s="80"/>
+      <c r="BG3" s="80"/>
+      <c r="BH3" s="80"/>
+      <c r="BI3" s="80"/>
+      <c r="BJ3" s="80"/>
+      <c r="BK3" s="80"/>
+      <c r="BL3" s="80"/>
+      <c r="BM3" s="80"/>
+      <c r="BN3" s="80"/>
+      <c r="BO3" s="80"/>
+      <c r="BP3" s="80"/>
+      <c r="BQ3" s="80"/>
+      <c r="BR3" s="80"/>
+      <c r="BS3" s="80"/>
+    </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="82"/>
-      <c r="AE4" s="82"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="82"/>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="82"/>
-      <c r="AK4" s="82"/>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="82"/>
-      <c r="AO4" s="82"/>
-      <c r="AP4" s="82"/>
-      <c r="AQ4" s="82"/>
-      <c r="AR4" s="82"/>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="82"/>
-      <c r="AV4" s="82"/>
-      <c r="AW4" s="82"/>
-      <c r="AX4" s="82"/>
-      <c r="AY4" s="82"/>
-      <c r="AZ4" s="82"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="82"/>
-      <c r="BC4" s="82"/>
-      <c r="BD4" s="82"/>
-      <c r="BE4" s="82"/>
-      <c r="BF4" s="82"/>
-      <c r="BG4" s="82"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="82"/>
-      <c r="BJ4" s="82"/>
-      <c r="BK4" s="82"/>
-      <c r="BL4" s="82"/>
-      <c r="BM4" s="82"/>
-      <c r="BN4" s="82"/>
-      <c r="BO4" s="82"/>
-      <c r="BP4" s="82"/>
-      <c r="BQ4" s="82"/>
-      <c r="BR4" s="82"/>
-    </row>
-    <row r="5" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="91"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="91"/>
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="91"/>
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="91"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="91"/>
+      <c r="BN4" s="91"/>
+      <c r="BO4" s="91"/>
+      <c r="BP4" s="91"/>
+      <c r="BQ4" s="91"/>
+      <c r="BR4" s="91"/>
+      <c r="BS4" s="91"/>
+    </row>
+    <row r="5" spans="1:89" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:89" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="74" t="s">
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="74" t="s">
+      <c r="H6" s="82"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="75"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="74" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="75"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="74" t="s">
+      <c r="N6" s="82"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="74" t="s">
+      <c r="Q6" s="82"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="75"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="74" t="s">
+      <c r="T6" s="82"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="75"/>
-      <c r="W6" s="76"/>
-      <c r="X6" s="74" t="s">
+      <c r="W6" s="82"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="76"/>
-      <c r="AA6" s="74" t="s">
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="76"/>
-      <c r="AD6" s="74" t="s">
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="AE6" s="75"/>
-      <c r="AF6" s="76"/>
-      <c r="AG6" s="74" t="s">
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="75"/>
-      <c r="AI6" s="76"/>
-      <c r="AJ6" s="74" t="s">
+      <c r="AI6" s="82"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="AK6" s="75"/>
-      <c r="AL6" s="76"/>
-      <c r="AM6" s="74" t="s">
+      <c r="AL6" s="82"/>
+      <c r="AM6" s="83"/>
+      <c r="AN6" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="AN6" s="75"/>
-      <c r="AO6" s="81"/>
-      <c r="AP6" s="74" t="s">
+      <c r="AO6" s="82"/>
+      <c r="AP6" s="90"/>
+      <c r="AQ6" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="AQ6" s="75"/>
-      <c r="AR6" s="81"/>
-      <c r="AS6" s="74" t="s">
+      <c r="AR6" s="82"/>
+      <c r="AS6" s="90"/>
+      <c r="AT6" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="75"/>
-      <c r="AU6" s="81"/>
-      <c r="AV6" s="74" t="s">
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="90"/>
+      <c r="AW6" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="AW6" s="75"/>
-      <c r="AX6" s="81"/>
-      <c r="AY6" s="74" t="s">
+      <c r="AX6" s="82"/>
+      <c r="AY6" s="90"/>
+      <c r="AZ6" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="81"/>
-      <c r="BB6" s="74" t="s">
+      <c r="BA6" s="82"/>
+      <c r="BB6" s="90"/>
+      <c r="BC6" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="75"/>
-      <c r="BD6" s="81"/>
-      <c r="BE6" s="74" t="s">
+      <c r="BD6" s="82"/>
+      <c r="BE6" s="90"/>
+      <c r="BF6" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="BF6" s="75"/>
-      <c r="BG6" s="81"/>
-      <c r="BH6" s="74" t="s">
+      <c r="BG6" s="82"/>
+      <c r="BH6" s="90"/>
+      <c r="BI6" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="BI6" s="75"/>
-      <c r="BJ6" s="81"/>
-      <c r="BK6" s="74" t="s">
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="90"/>
+      <c r="BL6" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="BL6" s="75"/>
-      <c r="BM6" s="81"/>
-      <c r="BN6" s="74" t="s">
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="90"/>
+      <c r="BO6" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="BO6" s="75"/>
-      <c r="BP6" s="81"/>
-      <c r="BQ6" s="74" t="s">
+      <c r="BP6" s="82"/>
+      <c r="BQ6" s="90"/>
+      <c r="BR6" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="BR6" s="75"/>
-      <c r="BS6" s="81"/>
-      <c r="BT6" s="74" t="s">
+      <c r="BS6" s="82"/>
+      <c r="BT6" s="90"/>
+      <c r="BU6" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="BU6" s="75"/>
-      <c r="BV6" s="81"/>
-      <c r="BW6" s="74" t="s">
+      <c r="BV6" s="82"/>
+      <c r="BW6" s="90"/>
+      <c r="BX6" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="BX6" s="75"/>
-      <c r="BY6" s="81"/>
-      <c r="BZ6" s="74" t="s">
+      <c r="BY6" s="82"/>
+      <c r="BZ6" s="90"/>
+      <c r="CA6" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="CA6" s="75"/>
-      <c r="CB6" s="81"/>
-      <c r="CC6" s="74" t="s">
+      <c r="CB6" s="82"/>
+      <c r="CC6" s="90"/>
+      <c r="CD6" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="CD6" s="75"/>
-      <c r="CE6" s="81"/>
-      <c r="CF6" s="77" t="s">
+      <c r="CE6" s="82"/>
+      <c r="CF6" s="90"/>
+      <c r="CG6" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="CH6" s="82"/>
+      <c r="CI6" s="90"/>
+      <c r="CJ6" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="CG6" s="79" t="s">
+      <c r="CK6" s="88" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="35" t="s">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A7" s="93"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="35" t="s">
+      <c r="G7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="35" t="s">
+      <c r="J7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="35" t="s">
+      <c r="M7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="35" t="s">
+      <c r="P7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="T7" s="35" t="s">
+      <c r="S7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="U7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="35" t="s">
+      <c r="V7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z7" s="35" t="s">
+      <c r="Y7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="AA7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC7" s="35" t="s">
+      <c r="AB7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AD7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF7" s="35" t="s">
+      <c r="AE7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AG7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI7" s="35" t="s">
+      <c r="AH7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AJ7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL7" s="35" t="s">
+      <c r="AK7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AM7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO7" s="12" t="s">
+      <c r="AN7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AP7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ7" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="AR7" s="12" t="s">
+      <c r="AQ7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AS7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="AU7" s="12" t="s">
+      <c r="AT7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AV7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="AX7" s="12" t="s">
+      <c r="AW7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AY7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="BA7" s="12" t="s">
+      <c r="AZ7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BB7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BC7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="BD7" s="12" t="s">
+      <c r="BC7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BD7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BE7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BF7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="BG7" s="12" t="s">
+      <c r="BF7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BH7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BI7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="BJ7" s="12" t="s">
+      <c r="BI7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BK7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BL7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="BM7" s="12" t="s">
+      <c r="BL7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="BN7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BN7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BO7" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="BP7" s="12" t="s">
+      <c r="BO7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP7" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BQ7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BR7" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="BS7" s="12" t="s">
+      <c r="BR7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BS7" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="BT7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BT7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BU7" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="BV7" s="12" t="s">
+      <c r="BU7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BV7" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="BW7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BW7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="BX7" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="BY7" s="12" t="s">
+      <c r="BX7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BY7" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="BZ7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="CA7" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="CB7" s="12" t="s">
+      <c r="CA7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="CB7" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="CC7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CC7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="CD7" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="CE7" s="12" t="s">
+      <c r="CD7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="CE7" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="CF7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CF7" s="78"/>
-      <c r="CG7" s="80"/>
-    </row>
-    <row r="8" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="CG7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="CH7" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="CI7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="CJ7" s="87"/>
+      <c r="CK7" s="89"/>
+    </row>
+    <row r="8" spans="1:89" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
       <c r="B8" s="58"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="33"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="33"/>
-      <c r="AB8" s="27"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="33"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="36"/>
-      <c r="AG8" s="33"/>
-      <c r="AH8" s="27"/>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="33"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="36"/>
-      <c r="AM8" s="33"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="28"/>
-      <c r="AP8" s="33"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="28"/>
-      <c r="AS8" s="33"/>
-      <c r="AT8" s="27"/>
-      <c r="AU8" s="28"/>
-      <c r="AV8" s="33"/>
-      <c r="AW8" s="27"/>
-      <c r="AX8" s="28"/>
-      <c r="AY8" s="33"/>
-      <c r="AZ8" s="27"/>
-      <c r="BA8" s="28"/>
-      <c r="BB8" s="33"/>
-      <c r="BC8" s="27"/>
-      <c r="BD8" s="28"/>
-      <c r="BE8" s="33"/>
-      <c r="BF8" s="27"/>
-      <c r="BG8" s="28"/>
-      <c r="BH8" s="33"/>
-      <c r="BI8" s="27"/>
-      <c r="BJ8" s="28"/>
-      <c r="BK8" s="33"/>
-      <c r="BL8" s="27"/>
-      <c r="BM8" s="28"/>
-      <c r="BN8" s="33"/>
-      <c r="BO8" s="27"/>
-      <c r="BP8" s="28"/>
-      <c r="BQ8" s="33"/>
-      <c r="BR8" s="27"/>
-      <c r="BS8" s="28"/>
-      <c r="BT8" s="33"/>
-      <c r="BU8" s="27"/>
-      <c r="BV8" s="28"/>
-      <c r="BW8" s="33"/>
-      <c r="BX8" s="27"/>
-      <c r="BY8" s="28"/>
-      <c r="BZ8" s="33"/>
-      <c r="CA8" s="27"/>
-      <c r="CB8" s="28"/>
-      <c r="CC8" s="33"/>
-      <c r="CD8" s="27"/>
-      <c r="CE8" s="28"/>
-      <c r="CF8" s="55"/>
-      <c r="CG8" s="45"/>
-    </row>
-    <row r="9" spans="1:85" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="58"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="33"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="33"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="33"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="36"/>
+      <c r="AK8" s="33"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="36"/>
+      <c r="AN8" s="33"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="28"/>
+      <c r="AQ8" s="33"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="33"/>
+      <c r="AU8" s="27"/>
+      <c r="AV8" s="28"/>
+      <c r="AW8" s="33"/>
+      <c r="AX8" s="27"/>
+      <c r="AY8" s="28"/>
+      <c r="AZ8" s="33"/>
+      <c r="BA8" s="27"/>
+      <c r="BB8" s="28"/>
+      <c r="BC8" s="33"/>
+      <c r="BD8" s="27"/>
+      <c r="BE8" s="28"/>
+      <c r="BF8" s="33"/>
+      <c r="BG8" s="27"/>
+      <c r="BH8" s="28"/>
+      <c r="BI8" s="33"/>
+      <c r="BJ8" s="27"/>
+      <c r="BK8" s="28"/>
+      <c r="BL8" s="33"/>
+      <c r="BM8" s="27"/>
+      <c r="BN8" s="28"/>
+      <c r="BO8" s="33"/>
+      <c r="BP8" s="27"/>
+      <c r="BQ8" s="28"/>
+      <c r="BR8" s="33"/>
+      <c r="BS8" s="27"/>
+      <c r="BT8" s="28"/>
+      <c r="BU8" s="33"/>
+      <c r="BV8" s="27"/>
+      <c r="BW8" s="28"/>
+      <c r="BX8" s="33"/>
+      <c r="BY8" s="27"/>
+      <c r="BZ8" s="28"/>
+      <c r="CA8" s="33"/>
+      <c r="CB8" s="27"/>
+      <c r="CC8" s="28"/>
+      <c r="CD8" s="72"/>
+      <c r="CE8" s="72"/>
+      <c r="CF8" s="72"/>
+      <c r="CG8" s="33"/>
+      <c r="CH8" s="27"/>
+      <c r="CI8" s="28"/>
+      <c r="CJ8" s="55"/>
+      <c r="CK8" s="45"/>
+    </row>
+    <row r="9" spans="1:89" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="31"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="37"/>
-      <c r="AD9" s="34"/>
-      <c r="AE9" s="29"/>
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="29"/>
-      <c r="AI9" s="37"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="29"/>
-      <c r="AL9" s="37"/>
-      <c r="AM9" s="34"/>
-      <c r="AN9" s="29"/>
-      <c r="AO9" s="30"/>
-      <c r="AP9" s="34"/>
-      <c r="AQ9" s="29"/>
-      <c r="AR9" s="30"/>
-      <c r="AS9" s="34"/>
-      <c r="AT9" s="29"/>
-      <c r="AU9" s="30"/>
-      <c r="AV9" s="34"/>
-      <c r="AW9" s="29"/>
-      <c r="AX9" s="30"/>
-      <c r="AY9" s="34"/>
-      <c r="AZ9" s="29"/>
-      <c r="BA9" s="30"/>
-      <c r="BB9" s="34"/>
-      <c r="BC9" s="29"/>
-      <c r="BD9" s="30"/>
-      <c r="BE9" s="34"/>
-      <c r="BF9" s="29"/>
-      <c r="BG9" s="30"/>
-      <c r="BH9" s="34"/>
-      <c r="BI9" s="29"/>
-      <c r="BJ9" s="30"/>
-      <c r="BK9" s="34"/>
-      <c r="BL9" s="29"/>
-      <c r="BM9" s="30"/>
-      <c r="BN9" s="34"/>
-      <c r="BO9" s="29"/>
-      <c r="BP9" s="30"/>
-      <c r="BQ9" s="34"/>
-      <c r="BR9" s="29"/>
-      <c r="BS9" s="30"/>
-      <c r="BT9" s="34"/>
-      <c r="BU9" s="29"/>
-      <c r="BV9" s="30"/>
-      <c r="BW9" s="34"/>
-      <c r="BX9" s="29"/>
-      <c r="BY9" s="30"/>
-      <c r="BZ9" s="34"/>
-      <c r="CA9" s="29"/>
-      <c r="CB9" s="30"/>
-      <c r="CC9" s="34"/>
-      <c r="CD9" s="29"/>
-      <c r="CE9" s="30"/>
-      <c r="CF9" s="56"/>
-    </row>
-    <row r="10" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="37"/>
+      <c r="AK9" s="34"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="37"/>
+      <c r="AN9" s="34"/>
+      <c r="AO9" s="29"/>
+      <c r="AP9" s="30"/>
+      <c r="AQ9" s="34"/>
+      <c r="AR9" s="29"/>
+      <c r="AS9" s="30"/>
+      <c r="AT9" s="34"/>
+      <c r="AU9" s="29"/>
+      <c r="AV9" s="30"/>
+      <c r="AW9" s="34"/>
+      <c r="AX9" s="29"/>
+      <c r="AY9" s="30"/>
+      <c r="AZ9" s="34"/>
+      <c r="BA9" s="29"/>
+      <c r="BB9" s="30"/>
+      <c r="BC9" s="34"/>
+      <c r="BD9" s="29"/>
+      <c r="BE9" s="30"/>
+      <c r="BF9" s="34"/>
+      <c r="BG9" s="29"/>
+      <c r="BH9" s="30"/>
+      <c r="BI9" s="34"/>
+      <c r="BJ9" s="29"/>
+      <c r="BK9" s="30"/>
+      <c r="BL9" s="34"/>
+      <c r="BM9" s="29"/>
+      <c r="BN9" s="30"/>
+      <c r="BO9" s="34"/>
+      <c r="BP9" s="29"/>
+      <c r="BQ9" s="30"/>
+      <c r="BR9" s="34"/>
+      <c r="BS9" s="29"/>
+      <c r="BT9" s="30"/>
+      <c r="BU9" s="34"/>
+      <c r="BV9" s="29"/>
+      <c r="BW9" s="30"/>
+      <c r="BX9" s="34"/>
+      <c r="BY9" s="29"/>
+      <c r="BZ9" s="30"/>
+      <c r="CA9" s="34"/>
+      <c r="CB9" s="29"/>
+      <c r="CC9" s="30"/>
+      <c r="CD9" s="73"/>
+      <c r="CE9" s="73"/>
+      <c r="CF9" s="73"/>
+      <c r="CG9" s="34"/>
+      <c r="CH9" s="29"/>
+      <c r="CI9" s="30"/>
+      <c r="CJ9" s="56"/>
+    </row>
+    <row r="10" spans="1:89" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -2382,7 +2460,7 @@
       <c r="R10" s="39"/>
       <c r="S10" s="39"/>
       <c r="T10" s="39"/>
-      <c r="U10" s="38"/>
+      <c r="U10" s="39"/>
       <c r="V10" s="38"/>
       <c r="W10" s="38"/>
       <c r="X10" s="38"/>
@@ -2403,54 +2481,56 @@
       <c r="AM10" s="38"/>
       <c r="AN10" s="38"/>
       <c r="AO10" s="38"/>
-    </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="AP10" s="38"/>
+    </row>
+    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
       <c r="L11" s="39"/>
       <c r="M11" s="39"/>
       <c r="N11" s="39"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="39"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="39"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="39"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="39"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="39"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="39"/>
-      <c r="AK11" s="38"/>
-      <c r="AL11" s="39"/>
-      <c r="AM11" s="38"/>
-      <c r="AN11" s="39"/>
-      <c r="AO11" s="38"/>
-    </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="O11" s="39"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="39"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="39"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="39"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="39"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="39"/>
+      <c r="AJ11" s="38"/>
+      <c r="AK11" s="39"/>
+      <c r="AL11" s="38"/>
+      <c r="AM11" s="39"/>
+      <c r="AN11" s="38"/>
+      <c r="AO11" s="39"/>
+      <c r="AP11" s="38"/>
+    </row>
+    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
@@ -2468,7 +2548,7 @@
       <c r="R12" s="39"/>
       <c r="S12" s="39"/>
       <c r="T12" s="39"/>
-      <c r="U12" s="38"/>
+      <c r="U12" s="39"/>
       <c r="V12" s="38"/>
       <c r="W12" s="38"/>
       <c r="X12" s="38"/>
@@ -2489,11 +2569,12 @@
       <c r="AM12" s="38"/>
       <c r="AN12" s="38"/>
       <c r="AO12" s="38"/>
-    </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="AP12" s="38"/>
+    </row>
+    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
@@ -2511,7 +2592,7 @@
       <c r="R13" s="39"/>
       <c r="S13" s="39"/>
       <c r="T13" s="39"/>
-      <c r="U13" s="38"/>
+      <c r="U13" s="39"/>
       <c r="V13" s="38"/>
       <c r="W13" s="38"/>
       <c r="X13" s="38"/>
@@ -2532,11 +2613,12 @@
       <c r="AM13" s="38"/>
       <c r="AN13" s="38"/>
       <c r="AO13" s="38"/>
-    </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="AP13" s="38"/>
+    </row>
+    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="39"/>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
@@ -2554,7 +2636,7 @@
       <c r="R14" s="39"/>
       <c r="S14" s="39"/>
       <c r="T14" s="39"/>
-      <c r="U14" s="38"/>
+      <c r="U14" s="39"/>
       <c r="V14" s="38"/>
       <c r="W14" s="38"/>
       <c r="X14" s="38"/>
@@ -2575,11 +2657,12 @@
       <c r="AM14" s="38"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="38"/>
-    </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="AP14" s="38"/>
+    </row>
+    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="39"/>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
@@ -2597,7 +2680,7 @@
       <c r="R15" s="39"/>
       <c r="S15" s="39"/>
       <c r="T15" s="39"/>
-      <c r="U15" s="38"/>
+      <c r="U15" s="39"/>
       <c r="V15" s="38"/>
       <c r="W15" s="38"/>
       <c r="X15" s="38"/>
@@ -2618,11 +2701,12 @@
       <c r="AM15" s="38"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="38"/>
-    </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="AP15" s="38"/>
+    </row>
+    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -2640,7 +2724,7 @@
       <c r="R16" s="39"/>
       <c r="S16" s="39"/>
       <c r="T16" s="39"/>
-      <c r="U16" s="38"/>
+      <c r="U16" s="39"/>
       <c r="V16" s="38"/>
       <c r="W16" s="38"/>
       <c r="X16" s="38"/>
@@ -2661,11 +2745,12 @@
       <c r="AM16" s="38"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="38"/>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP16" s="38"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
@@ -2683,7 +2768,7 @@
       <c r="R17" s="39"/>
       <c r="S17" s="39"/>
       <c r="T17" s="39"/>
-      <c r="U17" s="38"/>
+      <c r="U17" s="39"/>
       <c r="V17" s="38"/>
       <c r="W17" s="38"/>
       <c r="X17" s="38"/>
@@ -2704,11 +2789,12 @@
       <c r="AM17" s="38"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="38"/>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP17" s="38"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
@@ -2726,7 +2812,7 @@
       <c r="R18" s="39"/>
       <c r="S18" s="39"/>
       <c r="T18" s="39"/>
-      <c r="U18" s="38"/>
+      <c r="U18" s="39"/>
       <c r="V18" s="38"/>
       <c r="W18" s="38"/>
       <c r="X18" s="38"/>
@@ -2747,11 +2833,12 @@
       <c r="AM18" s="38"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="38"/>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP18" s="38"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
@@ -2769,7 +2856,7 @@
       <c r="R19" s="39"/>
       <c r="S19" s="39"/>
       <c r="T19" s="39"/>
-      <c r="U19" s="38"/>
+      <c r="U19" s="39"/>
       <c r="V19" s="38"/>
       <c r="W19" s="38"/>
       <c r="X19" s="38"/>
@@ -2790,11 +2877,12 @@
       <c r="AM19" s="38"/>
       <c r="AN19" s="38"/>
       <c r="AO19" s="38"/>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP19" s="38"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
@@ -2812,7 +2900,7 @@
       <c r="R20" s="39"/>
       <c r="S20" s="39"/>
       <c r="T20" s="39"/>
-      <c r="U20" s="38"/>
+      <c r="U20" s="39"/>
       <c r="V20" s="38"/>
       <c r="W20" s="38"/>
       <c r="X20" s="38"/>
@@ -2833,11 +2921,12 @@
       <c r="AM20" s="38"/>
       <c r="AN20" s="38"/>
       <c r="AO20" s="38"/>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP20" s="38"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="39"/>
       <c r="E21" s="39"/>
       <c r="F21" s="39"/>
@@ -2855,7 +2944,7 @@
       <c r="R21" s="39"/>
       <c r="S21" s="39"/>
       <c r="T21" s="39"/>
-      <c r="U21" s="38"/>
+      <c r="U21" s="39"/>
       <c r="V21" s="38"/>
       <c r="W21" s="38"/>
       <c r="X21" s="38"/>
@@ -2876,11 +2965,12 @@
       <c r="AM21" s="38"/>
       <c r="AN21" s="38"/>
       <c r="AO21" s="38"/>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP21" s="38"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="39"/>
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
@@ -2898,7 +2988,7 @@
       <c r="R22" s="39"/>
       <c r="S22" s="39"/>
       <c r="T22" s="39"/>
-      <c r="U22" s="38"/>
+      <c r="U22" s="39"/>
       <c r="V22" s="38"/>
       <c r="W22" s="38"/>
       <c r="X22" s="38"/>
@@ -2919,51 +3009,54 @@
       <c r="AM22" s="38"/>
       <c r="AN22" s="38"/>
       <c r="AO22" s="38"/>
+      <c r="AP22" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="CC6:CE6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="A4:BR4"/>
+  <mergeCells count="36">
+    <mergeCell ref="CG6:CI6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="A4:BS4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="M6:O6"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="CF6:CF7"/>
-    <mergeCell ref="CG6:CG7"/>
-    <mergeCell ref="BT6:BV6"/>
-    <mergeCell ref="BN6:BP6"/>
-    <mergeCell ref="AM6:AO6"/>
-    <mergeCell ref="BQ6:BS6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="BK6:BM6"/>
-    <mergeCell ref="AS6:AU6"/>
-    <mergeCell ref="AV6:AX6"/>
-    <mergeCell ref="AY6:BA6"/>
-    <mergeCell ref="BB6:BD6"/>
-    <mergeCell ref="BE6:BG6"/>
-    <mergeCell ref="BH6:BJ6"/>
-    <mergeCell ref="BW6:BY6"/>
-    <mergeCell ref="BZ6:CB6"/>
-    <mergeCell ref="A1:BR1"/>
-    <mergeCell ref="A3:BR3"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="AJ6:AL6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="CJ6:CJ7"/>
+    <mergeCell ref="CK6:CK7"/>
+    <mergeCell ref="BU6:BW6"/>
+    <mergeCell ref="BO6:BQ6"/>
+    <mergeCell ref="AN6:AP6"/>
+    <mergeCell ref="BR6:BT6"/>
+    <mergeCell ref="AQ6:AS6"/>
+    <mergeCell ref="BL6:BN6"/>
+    <mergeCell ref="AT6:AV6"/>
+    <mergeCell ref="AW6:AY6"/>
+    <mergeCell ref="AZ6:BB6"/>
+    <mergeCell ref="BC6:BE6"/>
+    <mergeCell ref="BF6:BH6"/>
+    <mergeCell ref="BI6:BK6"/>
+    <mergeCell ref="BX6:BZ6"/>
+    <mergeCell ref="CA6:CC6"/>
+    <mergeCell ref="A1:BS1"/>
+    <mergeCell ref="A3:BS3"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AG6"/>
+    <mergeCell ref="AH6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
-  <conditionalFormatting sqref="CF8:CF9">
+  <conditionalFormatting sqref="CJ8:CJ9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="16" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="15" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2972,175 +3065,422 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="74"/>
+      <c r="D4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="D6" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="E6" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="F6" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="G6" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="69" t="s">
+      <c r="H6" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="69" t="s">
+      <c r="I6" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="69" t="s">
+      <c r="J6" s="69" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="68"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="68"/>
       <c r="G7" s="68"/>
       <c r="H7" s="68"/>
       <c r="I7" s="68"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="68"/>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="29"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="104"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="38"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="38"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="38"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="38"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="38"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="38"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView topLeftCell="Q1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="19" width="11.28515625" style="3" customWidth="1"/>
+    <col min="20" max="37" width="11.28515625" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="94"/>
+      <c r="AC1" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="94"/>
+      <c r="AE1" s="94"/>
+      <c r="AF1" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="94"/>
+      <c r="AH1" s="94"/>
+      <c r="AI1" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ1" s="94"/>
+      <c r="AK1" s="94"/>
+      <c r="AL1" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" s="94"/>
+      <c r="AN1" s="94"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3165,66 +3505,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="72"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="79"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="87" t="s">
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="87" t="s">
+      <c r="J5" s="96"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="97"/>
     </row>
     <row r="6" spans="1:15" s="16" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -3354,232 +3694,6 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AN2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="19" width="11.28515625" style="3" customWidth="1"/>
-    <col min="20" max="37" width="11.28515625" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91"/>
-      <c r="AF1" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="91"/>
-      <c r="AI1" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ1" s="91"/>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM1" s="91"/>
-      <c r="AN1" s="91"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3617,92 +3731,98 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61B72FE-9BBD-48F6-9138-132EDBC73A96}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="63" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="63" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="63" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="63" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="63" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="63" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="63" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="63" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="92" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="101"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="62" t="s">
-        <v>5</v>
+      <c r="C6" s="75" t="s">
+        <v>79</v>
       </c>
       <c r="D6" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="62" t="s">
-        <v>6</v>
-      </c>
       <c r="F6" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="62" t="s">
+      <c r="H6" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="62" t="s">
+      <c r="I6" s="62" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
-      <c r="C7" s="65"/>
+      <c r="C7" s="64"/>
       <c r="D7" s="65"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="38"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dane - Salary Temp / Sales Report changes
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dane Burts\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B28C00C-983D-4D25-9C2E-0C275E977641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D39AA3E-1781-4F53-9F10-1D0E078F0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>She Macc Lite</t>
   </si>
   <si>
-    <t>Macc Fun R99</t>
-  </si>
-  <si>
     <t>Cancer R99</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>Cancer Spouse</t>
+  </si>
+  <si>
+    <t>Macc R99</t>
   </si>
 </sst>
 </file>
@@ -285,9 +285,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -946,7 +946,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -991,9 +991,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1103,14 +1103,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1124,7 +1124,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1141,89 +1141,89 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1585,422 +1585,422 @@
   </sheetPr>
   <dimension ref="A1:CK22"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="BL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BX6" sqref="BX6:BZ6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BL2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CA6" sqref="CA6:CC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="21" width="10.28515625" style="3" customWidth="1"/>
-    <col min="22" max="42" width="10.28515625" customWidth="1"/>
-    <col min="43" max="43" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="21" width="10.26953125" style="3" customWidth="1"/>
+    <col min="22" max="42" width="10.26953125" customWidth="1"/>
+    <col min="43" max="43" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="10" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="10" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="10" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="10" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="10" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.7109375" customWidth="1"/>
+    <col min="71" max="71" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:89" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
-      <c r="AG1" s="78"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="78"/>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="78"/>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="78"/>
-      <c r="AU1" s="78"/>
-      <c r="AV1" s="78"/>
-      <c r="AW1" s="78"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="78"/>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="78"/>
-      <c r="BB1" s="78"/>
-      <c r="BC1" s="78"/>
-      <c r="BD1" s="78"/>
-      <c r="BE1" s="78"/>
-      <c r="BF1" s="78"/>
-      <c r="BG1" s="78"/>
-      <c r="BH1" s="78"/>
-      <c r="BI1" s="78"/>
-      <c r="BJ1" s="78"/>
-      <c r="BK1" s="78"/>
-      <c r="BL1" s="78"/>
-      <c r="BM1" s="78"/>
-      <c r="BN1" s="78"/>
-      <c r="BO1" s="78"/>
-      <c r="BP1" s="78"/>
-      <c r="BQ1" s="78"/>
-      <c r="BR1" s="78"/>
-      <c r="BS1" s="79"/>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="95"/>
+      <c r="AC1" s="95"/>
+      <c r="AD1" s="95"/>
+      <c r="AE1" s="95"/>
+      <c r="AF1" s="95"/>
+      <c r="AG1" s="95"/>
+      <c r="AH1" s="95"/>
+      <c r="AI1" s="95"/>
+      <c r="AJ1" s="95"/>
+      <c r="AK1" s="95"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="95"/>
+      <c r="AP1" s="95"/>
+      <c r="AQ1" s="95"/>
+      <c r="AR1" s="95"/>
+      <c r="AS1" s="95"/>
+      <c r="AT1" s="95"/>
+      <c r="AU1" s="95"/>
+      <c r="AV1" s="95"/>
+      <c r="AW1" s="95"/>
+      <c r="AX1" s="95"/>
+      <c r="AY1" s="95"/>
+      <c r="AZ1" s="95"/>
+      <c r="BA1" s="95"/>
+      <c r="BB1" s="95"/>
+      <c r="BC1" s="95"/>
+      <c r="BD1" s="95"/>
+      <c r="BE1" s="95"/>
+      <c r="BF1" s="95"/>
+      <c r="BG1" s="95"/>
+      <c r="BH1" s="95"/>
+      <c r="BI1" s="95"/>
+      <c r="BJ1" s="95"/>
+      <c r="BK1" s="95"/>
+      <c r="BL1" s="95"/>
+      <c r="BM1" s="95"/>
+      <c r="BN1" s="95"/>
+      <c r="BO1" s="95"/>
+      <c r="BP1" s="95"/>
+      <c r="BQ1" s="95"/>
+      <c r="BR1" s="95"/>
+      <c r="BS1" s="96"/>
+    </row>
+    <row r="3" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="80"/>
-      <c r="U3" s="80"/>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="80"/>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="80"/>
-      <c r="AC3" s="80"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="80"/>
-      <c r="AH3" s="80"/>
-      <c r="AI3" s="80"/>
-      <c r="AJ3" s="80"/>
-      <c r="AK3" s="80"/>
-      <c r="AL3" s="80"/>
-      <c r="AM3" s="80"/>
-      <c r="AN3" s="80"/>
-      <c r="AO3" s="80"/>
-      <c r="AP3" s="80"/>
-      <c r="AQ3" s="80"/>
-      <c r="AR3" s="80"/>
-      <c r="AS3" s="80"/>
-      <c r="AT3" s="80"/>
-      <c r="AU3" s="80"/>
-      <c r="AV3" s="80"/>
-      <c r="AW3" s="80"/>
-      <c r="AX3" s="80"/>
-      <c r="AY3" s="80"/>
-      <c r="AZ3" s="80"/>
-      <c r="BA3" s="80"/>
-      <c r="BB3" s="80"/>
-      <c r="BC3" s="80"/>
-      <c r="BD3" s="80"/>
-      <c r="BE3" s="80"/>
-      <c r="BF3" s="80"/>
-      <c r="BG3" s="80"/>
-      <c r="BH3" s="80"/>
-      <c r="BI3" s="80"/>
-      <c r="BJ3" s="80"/>
-      <c r="BK3" s="80"/>
-      <c r="BL3" s="80"/>
-      <c r="BM3" s="80"/>
-      <c r="BN3" s="80"/>
-      <c r="BO3" s="80"/>
-      <c r="BP3" s="80"/>
-      <c r="BQ3" s="80"/>
-      <c r="BR3" s="80"/>
-      <c r="BS3" s="80"/>
-    </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="84"/>
+      <c r="AA3" s="84"/>
+      <c r="AB3" s="84"/>
+      <c r="AC3" s="84"/>
+      <c r="AD3" s="84"/>
+      <c r="AE3" s="84"/>
+      <c r="AF3" s="84"/>
+      <c r="AG3" s="84"/>
+      <c r="AH3" s="84"/>
+      <c r="AI3" s="84"/>
+      <c r="AJ3" s="84"/>
+      <c r="AK3" s="84"/>
+      <c r="AL3" s="84"/>
+      <c r="AM3" s="84"/>
+      <c r="AN3" s="84"/>
+      <c r="AO3" s="84"/>
+      <c r="AP3" s="84"/>
+      <c r="AQ3" s="84"/>
+      <c r="AR3" s="84"/>
+      <c r="AS3" s="84"/>
+      <c r="AT3" s="84"/>
+      <c r="AU3" s="84"/>
+      <c r="AV3" s="84"/>
+      <c r="AW3" s="84"/>
+      <c r="AX3" s="84"/>
+      <c r="AY3" s="84"/>
+      <c r="AZ3" s="84"/>
+      <c r="BA3" s="84"/>
+      <c r="BB3" s="84"/>
+      <c r="BC3" s="84"/>
+      <c r="BD3" s="84"/>
+      <c r="BE3" s="84"/>
+      <c r="BF3" s="84"/>
+      <c r="BG3" s="84"/>
+      <c r="BH3" s="84"/>
+      <c r="BI3" s="84"/>
+      <c r="BJ3" s="84"/>
+      <c r="BK3" s="84"/>
+      <c r="BL3" s="84"/>
+      <c r="BM3" s="84"/>
+      <c r="BN3" s="84"/>
+      <c r="BO3" s="84"/>
+      <c r="BP3" s="84"/>
+      <c r="BQ3" s="84"/>
+      <c r="BR3" s="84"/>
+      <c r="BS3" s="84"/>
+    </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="A4" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="91"/>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="91"/>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="91"/>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="91"/>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="91"/>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="91"/>
-      <c r="BN4" s="91"/>
-      <c r="BO4" s="91"/>
-      <c r="BP4" s="91"/>
-      <c r="BQ4" s="91"/>
-      <c r="BR4" s="91"/>
-      <c r="BS4" s="91"/>
-    </row>
-    <row r="5" spans="1:89" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:89" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92" t="s">
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="85"/>
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="85"/>
+      <c r="AK4" s="85"/>
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="85"/>
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="85"/>
+      <c r="AR4" s="85"/>
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="85"/>
+      <c r="AW4" s="85"/>
+      <c r="AX4" s="85"/>
+      <c r="AY4" s="85"/>
+      <c r="AZ4" s="85"/>
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="85"/>
+      <c r="BE4" s="85"/>
+      <c r="BF4" s="85"/>
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="85"/>
+      <c r="BM4" s="85"/>
+      <c r="BN4" s="85"/>
+      <c r="BO4" s="85"/>
+      <c r="BP4" s="85"/>
+      <c r="BQ4" s="85"/>
+      <c r="BR4" s="85"/>
+      <c r="BS4" s="85"/>
+    </row>
+    <row r="5" spans="1:89" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:89" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="81"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="81"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="81"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="81"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="81"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="W6" s="81"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="81"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF6" s="81"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="81"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL6" s="81"/>
+      <c r="AM6" s="83"/>
+      <c r="AN6" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO6" s="81"/>
+      <c r="AP6" s="82"/>
+      <c r="AQ6" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR6" s="81"/>
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU6" s="81"/>
+      <c r="AV6" s="82"/>
+      <c r="AW6" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX6" s="81"/>
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA6" s="81"/>
+      <c r="BB6" s="82"/>
+      <c r="BC6" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD6" s="81"/>
+      <c r="BE6" s="82"/>
+      <c r="BF6" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG6" s="81"/>
+      <c r="BH6" s="82"/>
+      <c r="BI6" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="BJ6" s="81"/>
+      <c r="BK6" s="82"/>
+      <c r="BL6" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="BM6" s="81"/>
+      <c r="BN6" s="82"/>
+      <c r="BO6" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="BP6" s="81"/>
+      <c r="BQ6" s="82"/>
+      <c r="BR6" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="BS6" s="81"/>
+      <c r="BT6" s="82"/>
+      <c r="BU6" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="BV6" s="81"/>
+      <c r="BW6" s="82"/>
+      <c r="BX6" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY6" s="81"/>
+      <c r="BZ6" s="82"/>
+      <c r="CA6" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="CB6" s="81"/>
+      <c r="CC6" s="82"/>
+      <c r="CD6" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="CE6" s="81"/>
+      <c r="CF6" s="82"/>
+      <c r="CG6" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="82"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="81" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="T6" s="82"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="W6" s="82"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC6" s="82"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF6" s="82"/>
-      <c r="AG6" s="83"/>
-      <c r="AH6" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI6" s="82"/>
-      <c r="AJ6" s="83"/>
-      <c r="AK6" s="81" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL6" s="82"/>
-      <c r="AM6" s="83"/>
-      <c r="AN6" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO6" s="82"/>
-      <c r="AP6" s="90"/>
-      <c r="AQ6" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="AR6" s="82"/>
-      <c r="AS6" s="90"/>
-      <c r="AT6" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="AU6" s="82"/>
-      <c r="AV6" s="90"/>
-      <c r="AW6" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX6" s="82"/>
-      <c r="AY6" s="90"/>
-      <c r="AZ6" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA6" s="82"/>
-      <c r="BB6" s="90"/>
-      <c r="BC6" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD6" s="82"/>
-      <c r="BE6" s="90"/>
-      <c r="BF6" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="BG6" s="82"/>
-      <c r="BH6" s="90"/>
-      <c r="BI6" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ6" s="82"/>
-      <c r="BK6" s="90"/>
-      <c r="BL6" s="81" t="s">
-        <v>48</v>
-      </c>
-      <c r="BM6" s="82"/>
-      <c r="BN6" s="90"/>
-      <c r="BO6" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="BP6" s="82"/>
-      <c r="BQ6" s="90"/>
-      <c r="BR6" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="BS6" s="82"/>
-      <c r="BT6" s="90"/>
-      <c r="BU6" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="BV6" s="82"/>
-      <c r="BW6" s="90"/>
-      <c r="BX6" s="81" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY6" s="82"/>
-      <c r="BZ6" s="90"/>
-      <c r="CA6" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB6" s="82"/>
-      <c r="CC6" s="90"/>
-      <c r="CD6" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="CE6" s="82"/>
-      <c r="CF6" s="90"/>
-      <c r="CG6" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="CH6" s="82"/>
-      <c r="CI6" s="90"/>
-      <c r="CJ6" s="86" t="s">
+      <c r="CH6" s="81"/>
+      <c r="CI6" s="82"/>
+      <c r="CJ6" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="CK6" s="88" t="s">
+      <c r="CK6" s="92" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
+    <row r="7" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="A7" s="89"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2253,10 +2253,10 @@
       <c r="CI7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CJ7" s="87"/>
-      <c r="CK7" s="89"/>
-    </row>
-    <row r="8" spans="1:89" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="CJ7" s="91"/>
+      <c r="CK7" s="93"/>
+    </row>
+    <row r="8" spans="1:89" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="57"/>
       <c r="B8" s="58"/>
       <c r="C8" s="58"/>
@@ -2347,7 +2347,7 @@
       <c r="CJ8" s="55"/>
       <c r="CK8" s="45"/>
     </row>
-    <row r="9" spans="1:89" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:89" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="CI9" s="30"/>
       <c r="CJ9" s="56"/>
     </row>
-    <row r="10" spans="1:89" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -2483,7 +2483,7 @@
       <c r="AO10" s="38"/>
       <c r="AP10" s="38"/>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2527,7 +2527,7 @@
       <c r="AO11" s="39"/>
       <c r="AP11" s="38"/>
     </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -2571,7 +2571,7 @@
       <c r="AO12" s="38"/>
       <c r="AP12" s="38"/>
     </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -2615,7 +2615,7 @@
       <c r="AO13" s="38"/>
       <c r="AP13" s="38"/>
     </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -2659,7 +2659,7 @@
       <c r="AO14" s="38"/>
       <c r="AP14" s="38"/>
     </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -2703,7 +2703,7 @@
       <c r="AO15" s="38"/>
       <c r="AP15" s="38"/>
     </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -2747,7 +2747,7 @@
       <c r="AO16" s="38"/>
       <c r="AP16" s="38"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -2791,7 +2791,7 @@
       <c r="AO17" s="38"/>
       <c r="AP17" s="38"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -2835,7 +2835,7 @@
       <c r="AO18" s="38"/>
       <c r="AP18" s="38"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -2879,7 +2879,7 @@
       <c r="AO19" s="38"/>
       <c r="AP19" s="38"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -2923,7 +2923,7 @@
       <c r="AO20" s="38"/>
       <c r="AP20" s="38"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
@@ -2967,7 +2967,7 @@
       <c r="AO21" s="38"/>
       <c r="AP21" s="38"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
@@ -3013,13 +3013,19 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="CG6:CI6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="A4:BS4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="A1:BS1"/>
+    <mergeCell ref="A3:BS3"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AG6"/>
+    <mergeCell ref="AH6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="CJ6:CJ7"/>
     <mergeCell ref="CK6:CK7"/>
     <mergeCell ref="BU6:BW6"/>
@@ -3036,19 +3042,13 @@
     <mergeCell ref="BI6:BK6"/>
     <mergeCell ref="BX6:BZ6"/>
     <mergeCell ref="CA6:CC6"/>
-    <mergeCell ref="A1:BS1"/>
-    <mergeCell ref="A3:BS3"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AG6"/>
-    <mergeCell ref="AH6:AJ6"/>
-    <mergeCell ref="AK6:AM6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="CG6:CI6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="A4:BS4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="CD6:CF6"/>
   </mergeCells>
   <conditionalFormatting sqref="CJ8:CJ9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -3071,55 +3071,55 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="1" max="2" width="28.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="79"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="43"/>
       <c r="B4" s="74"/>
       <c r="D4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="105" t="s">
-        <v>79</v>
+      <c r="B6" s="79" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>54</v>
@@ -3131,24 +3131,24 @@
         <v>46</v>
       </c>
       <c r="F6" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="69" t="s">
         <v>73</v>
-      </c>
-      <c r="G6" s="69" t="s">
-        <v>74</v>
       </c>
       <c r="H6" s="69" t="s">
         <v>69</v>
       </c>
       <c r="I6" s="69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J6" s="69" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13"/>
-      <c r="B7" s="103"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="47"/>
       <c r="D7" s="27"/>
       <c r="E7" s="53"/>
@@ -3158,87 +3158,87 @@
       <c r="I7" s="68"/>
       <c r="J7" s="68"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="104"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="48"/>
       <c r="D8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
@@ -3250,7 +3250,7 @@
     <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3260,84 +3260,84 @@
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="19" width="11.28515625" style="3" customWidth="1"/>
-    <col min="20" max="37" width="11.28515625" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="19" width="11.26953125" style="3" customWidth="1"/>
+    <col min="20" max="37" width="11.26953125" customWidth="1"/>
+    <col min="38" max="38" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94" t="s">
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94" t="s">
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94" t="s">
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94" t="s">
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94" t="s">
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94" t="s">
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="94"/>
-      <c r="Y1" s="94"/>
-      <c r="Z1" s="94" t="s">
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="94"/>
-      <c r="AB1" s="94"/>
-      <c r="AC1" s="94" t="s">
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="94"/>
-      <c r="AE1" s="94"/>
-      <c r="AF1" s="94" t="s">
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="94"/>
-      <c r="AH1" s="94"/>
-      <c r="AI1" s="94" t="s">
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="AJ1" s="94"/>
-      <c r="AK1" s="94"/>
-      <c r="AL1" s="94" t="s">
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" s="94"/>
-      <c r="AN1" s="94"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3491,82 +3491,82 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="95" t="s">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="95" t="s">
+      <c r="J5" s="99"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="97"/>
-    </row>
-    <row r="6" spans="1:15" s="16" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="100"/>
+    </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17"/>
       <c r="B7" s="13"/>
       <c r="C7" s="42"/>
@@ -3630,8 +3630,8 @@
       <c r="N7" s="18"/>
       <c r="O7" s="19"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3678,10 +3678,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E10" s="15"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C16" s="15"/>
     </row>
   </sheetData>
@@ -3705,14 +3705,14 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -3733,44 +3733,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61B72FE-9BBD-48F6-9138-132EDBC73A96}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="63" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="63" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="63" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="63" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" style="63" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="63" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="63" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" style="63" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+      <c r="A1" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" s="99" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D5" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="101"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="104"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>18</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>63</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="62" t="s">
         <v>5</v>
@@ -3793,13 +3793,13 @@
         <v>67</v>
       </c>
       <c r="H6" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="64"/>
@@ -3810,13 +3810,13 @@
       <c r="H7" s="71"/>
       <c r="I7" s="71"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H8" s="38"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H10" s="38"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temp Salary Adaptations - Dane
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateTempSalaryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dane Burts\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D39AA3E-1781-4F53-9F10-1D0E078F0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2969E501-6927-49BC-9210-94A8ACD2A81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="82">
   <si>
     <t xml:space="preserve">Cancer </t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Macc R99</t>
+  </si>
+  <si>
+    <t>Macc Spouse</t>
   </si>
 </sst>
 </file>
@@ -285,9 +288,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -946,9 +949,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -991,9 +994,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1103,14 +1106,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1124,7 +1127,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1147,22 +1150,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1171,33 +1180,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1213,13 +1219,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1583,113 +1589,113 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CK22"/>
+  <dimension ref="A1:CN22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BL2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CA6" sqref="CA6:CC6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BM2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CJ6" sqref="CJ6:CL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="3" width="20.54296875" customWidth="1"/>
-    <col min="4" max="21" width="10.26953125" style="3" customWidth="1"/>
-    <col min="22" max="42" width="10.26953125" customWidth="1"/>
-    <col min="43" max="43" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="21" width="10.28515625" style="3" customWidth="1"/>
+    <col min="22" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="10" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="10" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="10" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="10" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="10" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.7265625" customWidth="1"/>
+    <col min="71" max="71" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:92" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="95"/>
-      <c r="AB1" s="95"/>
-      <c r="AC1" s="95"/>
-      <c r="AD1" s="95"/>
-      <c r="AE1" s="95"/>
-      <c r="AF1" s="95"/>
-      <c r="AG1" s="95"/>
-      <c r="AH1" s="95"/>
-      <c r="AI1" s="95"/>
-      <c r="AJ1" s="95"/>
-      <c r="AK1" s="95"/>
-      <c r="AL1" s="95"/>
-      <c r="AM1" s="95"/>
-      <c r="AN1" s="95"/>
-      <c r="AO1" s="95"/>
-      <c r="AP1" s="95"/>
-      <c r="AQ1" s="95"/>
-      <c r="AR1" s="95"/>
-      <c r="AS1" s="95"/>
-      <c r="AT1" s="95"/>
-      <c r="AU1" s="95"/>
-      <c r="AV1" s="95"/>
-      <c r="AW1" s="95"/>
-      <c r="AX1" s="95"/>
-      <c r="AY1" s="95"/>
-      <c r="AZ1" s="95"/>
-      <c r="BA1" s="95"/>
-      <c r="BB1" s="95"/>
-      <c r="BC1" s="95"/>
-      <c r="BD1" s="95"/>
-      <c r="BE1" s="95"/>
-      <c r="BF1" s="95"/>
-      <c r="BG1" s="95"/>
-      <c r="BH1" s="95"/>
-      <c r="BI1" s="95"/>
-      <c r="BJ1" s="95"/>
-      <c r="BK1" s="95"/>
-      <c r="BL1" s="95"/>
-      <c r="BM1" s="95"/>
-      <c r="BN1" s="95"/>
-      <c r="BO1" s="95"/>
-      <c r="BP1" s="95"/>
-      <c r="BQ1" s="95"/>
-      <c r="BR1" s="95"/>
-      <c r="BS1" s="96"/>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="82"/>
+      <c r="AC1" s="82"/>
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="82"/>
+      <c r="AF1" s="82"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="82"/>
+      <c r="AI1" s="82"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="82"/>
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="82"/>
+      <c r="AN1" s="82"/>
+      <c r="AO1" s="82"/>
+      <c r="AP1" s="82"/>
+      <c r="AQ1" s="82"/>
+      <c r="AR1" s="82"/>
+      <c r="AS1" s="82"/>
+      <c r="AT1" s="82"/>
+      <c r="AU1" s="82"/>
+      <c r="AV1" s="82"/>
+      <c r="AW1" s="82"/>
+      <c r="AX1" s="82"/>
+      <c r="AY1" s="82"/>
+      <c r="AZ1" s="82"/>
+      <c r="BA1" s="82"/>
+      <c r="BB1" s="82"/>
+      <c r="BC1" s="82"/>
+      <c r="BD1" s="82"/>
+      <c r="BE1" s="82"/>
+      <c r="BF1" s="82"/>
+      <c r="BG1" s="82"/>
+      <c r="BH1" s="82"/>
+      <c r="BI1" s="82"/>
+      <c r="BJ1" s="82"/>
+      <c r="BK1" s="82"/>
+      <c r="BL1" s="82"/>
+      <c r="BM1" s="82"/>
+      <c r="BN1" s="82"/>
+      <c r="BO1" s="82"/>
+      <c r="BP1" s="82"/>
+      <c r="BQ1" s="82"/>
+      <c r="BR1" s="82"/>
+      <c r="BS1" s="83"/>
+    </row>
+    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
@@ -1764,243 +1770,248 @@
       <c r="BR3" s="84"/>
       <c r="BS3" s="84"/>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A4" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="85"/>
-      <c r="W4" s="85"/>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="85"/>
-      <c r="AD4" s="85"/>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="85"/>
-      <c r="AK4" s="85"/>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="85"/>
-      <c r="AO4" s="85"/>
-      <c r="AP4" s="85"/>
-      <c r="AQ4" s="85"/>
-      <c r="AR4" s="85"/>
-      <c r="AS4" s="85"/>
-      <c r="AT4" s="85"/>
-      <c r="AU4" s="85"/>
-      <c r="AV4" s="85"/>
-      <c r="AW4" s="85"/>
-      <c r="AX4" s="85"/>
-      <c r="AY4" s="85"/>
-      <c r="AZ4" s="85"/>
-      <c r="BA4" s="85"/>
-      <c r="BB4" s="85"/>
-      <c r="BC4" s="85"/>
-      <c r="BD4" s="85"/>
-      <c r="BE4" s="85"/>
-      <c r="BF4" s="85"/>
-      <c r="BG4" s="85"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="85"/>
-      <c r="BJ4" s="85"/>
-      <c r="BK4" s="85"/>
-      <c r="BL4" s="85"/>
-      <c r="BM4" s="85"/>
-      <c r="BN4" s="85"/>
-      <c r="BO4" s="85"/>
-      <c r="BP4" s="85"/>
-      <c r="BQ4" s="85"/>
-      <c r="BR4" s="85"/>
-      <c r="BS4" s="85"/>
-    </row>
-    <row r="5" spans="1:89" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:89" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="88" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="95"/>
+      <c r="X4" s="95"/>
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="95"/>
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="95"/>
+      <c r="AS4" s="95"/>
+      <c r="AT4" s="95"/>
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="95"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="95"/>
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="95"/>
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="95"/>
+      <c r="BG4" s="95"/>
+      <c r="BH4" s="95"/>
+      <c r="BI4" s="95"/>
+      <c r="BJ4" s="95"/>
+      <c r="BK4" s="95"/>
+      <c r="BL4" s="95"/>
+      <c r="BM4" s="95"/>
+      <c r="BN4" s="95"/>
+      <c r="BO4" s="95"/>
+      <c r="BP4" s="95"/>
+      <c r="BQ4" s="95"/>
+      <c r="BR4" s="95"/>
+      <c r="BS4" s="95"/>
+    </row>
+    <row r="5" spans="1:92" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:92" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="80" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="81"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="80" t="s">
+      <c r="H6" s="86"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="80" t="s">
+      <c r="K6" s="86"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="81"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="80" t="s">
+      <c r="N6" s="86"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="80" t="s">
+      <c r="Q6" s="86"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="81"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="80" t="s">
+      <c r="T6" s="86"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="W6" s="81"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="80" t="s">
+      <c r="W6" s="86"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="81"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="80" t="s">
+      <c r="Z6" s="86"/>
+      <c r="AA6" s="87"/>
+      <c r="AB6" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="81"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="80" t="s">
+      <c r="AC6" s="86"/>
+      <c r="AD6" s="87"/>
+      <c r="AE6" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="AF6" s="81"/>
-      <c r="AG6" s="83"/>
-      <c r="AH6" s="80" t="s">
+      <c r="AF6" s="86"/>
+      <c r="AG6" s="87"/>
+      <c r="AH6" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="AI6" s="81"/>
-      <c r="AJ6" s="83"/>
-      <c r="AK6" s="80" t="s">
+      <c r="AI6" s="86"/>
+      <c r="AJ6" s="87"/>
+      <c r="AK6" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="AL6" s="81"/>
-      <c r="AM6" s="83"/>
-      <c r="AN6" s="80" t="s">
+      <c r="AL6" s="86"/>
+      <c r="AM6" s="87"/>
+      <c r="AN6" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="AO6" s="81"/>
-      <c r="AP6" s="82"/>
-      <c r="AQ6" s="80" t="s">
+      <c r="AO6" s="86"/>
+      <c r="AP6" s="94"/>
+      <c r="AQ6" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="AR6" s="81"/>
-      <c r="AS6" s="82"/>
-      <c r="AT6" s="80" t="s">
+      <c r="AR6" s="86"/>
+      <c r="AS6" s="94"/>
+      <c r="AT6" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="AU6" s="81"/>
-      <c r="AV6" s="82"/>
-      <c r="AW6" s="80" t="s">
+      <c r="AU6" s="86"/>
+      <c r="AV6" s="94"/>
+      <c r="AW6" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="AX6" s="81"/>
-      <c r="AY6" s="82"/>
-      <c r="AZ6" s="80" t="s">
+      <c r="AX6" s="86"/>
+      <c r="AY6" s="94"/>
+      <c r="AZ6" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="BA6" s="81"/>
-      <c r="BB6" s="82"/>
-      <c r="BC6" s="80" t="s">
+      <c r="BA6" s="86"/>
+      <c r="BB6" s="94"/>
+      <c r="BC6" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="BD6" s="81"/>
-      <c r="BE6" s="82"/>
-      <c r="BF6" s="80" t="s">
+      <c r="BD6" s="86"/>
+      <c r="BE6" s="94"/>
+      <c r="BF6" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="BG6" s="81"/>
-      <c r="BH6" s="82"/>
-      <c r="BI6" s="80" t="s">
+      <c r="BG6" s="86"/>
+      <c r="BH6" s="94"/>
+      <c r="BI6" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="BJ6" s="81"/>
-      <c r="BK6" s="82"/>
-      <c r="BL6" s="80" t="s">
+      <c r="BJ6" s="86"/>
+      <c r="BK6" s="94"/>
+      <c r="BL6" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="BM6" s="81"/>
-      <c r="BN6" s="82"/>
-      <c r="BO6" s="80" t="s">
+      <c r="BM6" s="86"/>
+      <c r="BN6" s="94"/>
+      <c r="BO6" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="BP6" s="81"/>
-      <c r="BQ6" s="82"/>
-      <c r="BR6" s="80" t="s">
+      <c r="BP6" s="86"/>
+      <c r="BQ6" s="94"/>
+      <c r="BR6" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="BS6" s="81"/>
-      <c r="BT6" s="82"/>
-      <c r="BU6" s="80" t="s">
+      <c r="BS6" s="86"/>
+      <c r="BT6" s="94"/>
+      <c r="BU6" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="BV6" s="81"/>
-      <c r="BW6" s="82"/>
-      <c r="BX6" s="80" t="s">
+      <c r="BV6" s="86"/>
+      <c r="BW6" s="94"/>
+      <c r="BX6" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="BY6" s="81"/>
-      <c r="BZ6" s="82"/>
-      <c r="CA6" s="80" t="s">
+      <c r="BY6" s="86"/>
+      <c r="BZ6" s="94"/>
+      <c r="CA6" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="CB6" s="81"/>
-      <c r="CC6" s="82"/>
-      <c r="CD6" s="80" t="s">
+      <c r="CB6" s="86"/>
+      <c r="CC6" s="94"/>
+      <c r="CD6" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="CE6" s="81"/>
-      <c r="CF6" s="82"/>
-      <c r="CG6" s="80" t="s">
+      <c r="CE6" s="86"/>
+      <c r="CF6" s="94"/>
+      <c r="CG6" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="CH6" s="81"/>
-      <c r="CI6" s="82"/>
-      <c r="CJ6" s="90" t="s">
+      <c r="CH6" s="86"/>
+      <c r="CI6" s="94"/>
+      <c r="CJ6" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="CK6" s="86"/>
+      <c r="CL6" s="94"/>
+      <c r="CM6" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="CK6" s="92" t="s">
+      <c r="CN6" s="92" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A7" s="89"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+    <row r="7" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A7" s="97"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
       <c r="D7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2253,10 +2264,19 @@
       <c r="CI7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="CJ7" s="91"/>
-      <c r="CK7" s="93"/>
-    </row>
-    <row r="8" spans="1:89" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="CJ7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="CK7" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="CL7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="CM7" s="91"/>
+      <c r="CN7" s="93"/>
+    </row>
+    <row r="8" spans="1:92" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
       <c r="B8" s="58"/>
       <c r="C8" s="58"/>
@@ -2344,10 +2364,13 @@
       <c r="CG8" s="33"/>
       <c r="CH8" s="27"/>
       <c r="CI8" s="28"/>
-      <c r="CJ8" s="55"/>
-      <c r="CK8" s="45"/>
-    </row>
-    <row r="9" spans="1:89" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="CJ8" s="33"/>
+      <c r="CK8" s="27"/>
+      <c r="CL8" s="28"/>
+      <c r="CM8" s="55"/>
+      <c r="CN8" s="45"/>
+    </row>
+    <row r="9" spans="1:92" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
@@ -2437,9 +2460,12 @@
       <c r="CG9" s="34"/>
       <c r="CH9" s="29"/>
       <c r="CI9" s="30"/>
-      <c r="CJ9" s="56"/>
-    </row>
-    <row r="10" spans="1:89" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="CJ9" s="34"/>
+      <c r="CK9" s="29"/>
+      <c r="CL9" s="30"/>
+      <c r="CM9" s="56"/>
+    </row>
+    <row r="10" spans="1:92" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -2483,7 +2509,7 @@
       <c r="AO10" s="38"/>
       <c r="AP10" s="38"/>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2527,7 +2553,7 @@
       <c r="AO11" s="39"/>
       <c r="AP11" s="38"/>
     </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -2571,7 +2597,7 @@
       <c r="AO12" s="38"/>
       <c r="AP12" s="38"/>
     </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -2615,7 +2641,7 @@
       <c r="AO13" s="38"/>
       <c r="AP13" s="38"/>
     </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -2659,7 +2685,7 @@
       <c r="AO14" s="38"/>
       <c r="AP14" s="38"/>
     </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -2703,7 +2729,7 @@
       <c r="AO15" s="38"/>
       <c r="AP15" s="38"/>
     </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -2747,7 +2773,7 @@
       <c r="AO16" s="38"/>
       <c r="AP16" s="38"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -2791,7 +2817,7 @@
       <c r="AO17" s="38"/>
       <c r="AP17" s="38"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -2835,7 +2861,7 @@
       <c r="AO18" s="38"/>
       <c r="AP18" s="38"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -2879,7 +2905,7 @@
       <c r="AO19" s="38"/>
       <c r="AP19" s="38"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -2923,7 +2949,7 @@
       <c r="AO20" s="38"/>
       <c r="AP20" s="38"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
@@ -2967,7 +2993,7 @@
       <c r="AO21" s="38"/>
       <c r="AP21" s="38"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
@@ -3012,22 +3038,17 @@
       <c r="AP22" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A1:BS1"/>
-    <mergeCell ref="A3:BS3"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AG6"/>
-    <mergeCell ref="AH6:AJ6"/>
-    <mergeCell ref="AK6:AM6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="CJ6:CJ7"/>
-    <mergeCell ref="CK6:CK7"/>
+  <mergeCells count="37">
+    <mergeCell ref="CJ6:CL6"/>
+    <mergeCell ref="CG6:CI6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="A4:BS4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="CM6:CM7"/>
+    <mergeCell ref="CN6:CN7"/>
     <mergeCell ref="BU6:BW6"/>
     <mergeCell ref="BO6:BQ6"/>
     <mergeCell ref="AN6:AP6"/>
@@ -3042,21 +3063,27 @@
     <mergeCell ref="BI6:BK6"/>
     <mergeCell ref="BX6:BZ6"/>
     <mergeCell ref="CA6:CC6"/>
-    <mergeCell ref="CG6:CI6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="A4:BS4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="A1:BS1"/>
+    <mergeCell ref="A3:BS3"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AG6"/>
+    <mergeCell ref="AH6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
-  <conditionalFormatting sqref="CJ8:CJ9">
+  <conditionalFormatting sqref="CM8:CM9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="15" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="14" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3071,30 +3098,30 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="28.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="1" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="96"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="83"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
@@ -3107,14 +3134,14 @@
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="74"/>
       <c r="D4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>18</v>
       </c>
@@ -3146,7 +3173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="77"/>
       <c r="C7" s="47"/>
@@ -3158,7 +3185,7 @@
       <c r="I7" s="68"/>
       <c r="J7" s="68"/>
     </row>
-    <row r="8" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
@@ -3166,79 +3193,79 @@
       <c r="C8" s="48"/>
       <c r="D8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
@@ -3250,7 +3277,7 @@
     <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3260,84 +3287,84 @@
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="19" width="11.26953125" style="3" customWidth="1"/>
-    <col min="20" max="37" width="11.26953125" customWidth="1"/>
-    <col min="38" max="38" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="19" width="11.28515625" style="3" customWidth="1"/>
+    <col min="20" max="37" width="11.28515625" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97" t="s">
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97" t="s">
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97" t="s">
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97" t="s">
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97" t="s">
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97" t="s">
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97" t="s">
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97" t="s">
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="97"/>
-      <c r="AE1" s="97"/>
-      <c r="AF1" s="97" t="s">
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="97"/>
-      <c r="AH1" s="97"/>
-      <c r="AI1" s="97" t="s">
+      <c r="AG1" s="98"/>
+      <c r="AH1" s="98"/>
+      <c r="AI1" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="AJ1" s="97"/>
-      <c r="AK1" s="97"/>
-      <c r="AL1" s="97" t="s">
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="98"/>
+      <c r="AL1" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" s="97"/>
-      <c r="AN1" s="97"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM1" s="98"/>
+      <c r="AN1" s="98"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3491,39 +3518,39 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11.453125" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="96"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="83"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="84" t="s">
         <v>40</v>
       </c>
@@ -3542,31 +3569,31 @@
       <c r="N3" s="84"/>
       <c r="O3" s="84"/>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="98" t="s">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="98" t="s">
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="99"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="98" t="s">
+      <c r="J5" s="100"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="100"/>
-    </row>
-    <row r="6" spans="1:15" s="16" customFormat="1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="101"/>
+    </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
@@ -3613,7 +3640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="13"/>
       <c r="C7" s="42"/>
@@ -3630,8 +3657,8 @@
       <c r="N7" s="18"/>
       <c r="O7" s="19"/>
     </row>
-    <row r="8" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3678,10 +3705,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10" s="15"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="15"/>
     </row>
   </sheetData>
@@ -3705,14 +3732,14 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -3737,40 +3764,40 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="24.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" style="63" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="63" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="63" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" style="63" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="63" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="63" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="63" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="63" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D5" s="102" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="104"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="105"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>18</v>
       </c>
@@ -3799,7 +3826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="64"/>
@@ -3810,13 +3837,13 @@
       <c r="H7" s="71"/>
       <c r="I7" s="71"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H8" s="38"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H10" s="38"/>
     </row>
   </sheetData>

</xml_diff>